<commit_message>
Correction of ELCCO2 COA - Supposed to be NGA
</commit_message>
<xml_diff>
--- a/VT_SHR_ELC_V01.xlsx
+++ b/VT_SHR_ELC_V01.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="9555" yWindow="-15" windowWidth="4125" windowHeight="9405" tabRatio="901" activeTab="2"/>
+    <workbookView xWindow="9555" yWindow="-15" windowWidth="4125" windowHeight="9405" tabRatio="901" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="SEC_Comm" sheetId="112" r:id="rId1"/>
@@ -1420,10 +1420,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
-    <numFmt numFmtId="200" formatCode="0.0000"/>
-    <numFmt numFmtId="201" formatCode="\Te\x\t"/>
+    <numFmt numFmtId="164" formatCode="0.0000"/>
+    <numFmt numFmtId="165" formatCode="\Te\x\t"/>
   </numFmts>
-  <fonts count="22" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1493,12 +1493,6 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="8"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="12"/>
       <color indexed="53"/>
       <name val="Arial"/>
@@ -1513,28 +1507,8 @@
     </font>
     <font>
       <b/>
-      <sz val="8"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
       <sz val="14"/>
       <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="8"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
       <family val="2"/>
     </font>
     <font>
@@ -1716,8 +1690,8 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -1740,7 +1714,7 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="4" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="4" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="5"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="5" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="5" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1780,28 +1754,28 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="4" applyFont="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="4" applyFont="1"/>
     <xf numFmtId="1" fontId="4" fillId="8" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="2" fontId="4" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="201" fontId="3" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="201" fontId="7" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="201" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="201" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="201" fontId="2" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="201" fontId="2" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="201" fontId="2" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="3" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="7" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="2" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="2" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="2" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="201" fontId="4" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="4" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="201" fontId="4" fillId="2" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="4" fillId="2" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="201" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -1814,25 +1788,25 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="4" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="200" fontId="4" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="4" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="10" borderId="3" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="11" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -2841,7 +2815,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:V30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="O17" sqref="O17"/>
     </sheetView>
   </sheetViews>
@@ -3688,8 +3662,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A4:F12"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3721,7 +3695,7 @@
         <v>100</v>
       </c>
       <c r="D7" s="18" t="s">
-        <v>100</v>
+        <v>108</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
I removed the ProcessCharacterizationHorizontal since it is not used
</commit_message>
<xml_diff>
--- a/VT_SHR_ELC_V01.xlsx
+++ b/VT_SHR_ELC_V01.xlsx
@@ -5,21 +5,20 @@
   <workbookPr showObjects="placeholders" codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Mikkel Simonsen\TIMES-DK\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Najub\TIMES-Shire\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="9555" yWindow="-15" windowWidth="4125" windowHeight="9405" tabRatio="901" activeTab="4"/>
+    <workbookView xWindow="9552" yWindow="-12" windowWidth="4128" windowHeight="9408" tabRatio="901"/>
   </bookViews>
   <sheets>
     <sheet name="SEC_Comm" sheetId="112" r:id="rId1"/>
     <sheet name="SEC_Processes" sheetId="127" r:id="rId2"/>
     <sheet name="ProcessCharac" sheetId="132" r:id="rId3"/>
-    <sheet name="ProcessCharac_Horizontal" sheetId="131" r:id="rId4"/>
-    <sheet name="EmissionTable" sheetId="126" r:id="rId5"/>
+    <sheet name="EmissionTable" sheetId="126" r:id="rId4"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId6"/>
+    <externalReference r:id="rId5"/>
   </externalReferences>
   <definedNames>
     <definedName name="FID_1">[1]AGR_Fuels!$A$2</definedName>
@@ -851,103 +850,6 @@
     <author>Maurizio Gargiulo</author>
   </authors>
   <commentList>
-    <comment ref="C8" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>With this character *, this column is ignored from VEDA.
-It is just useful for your information</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="G8" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Allowed Lim Type</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-UP</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> (upper for &gt;=)</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-LO</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> (Lower for &lt;=)</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-FX</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> (Fix for =)</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
-<file path=xl/comments5.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <authors>
-    <author>Maurizio Gargiulo</author>
-  </authors>
-  <commentList>
     <comment ref="B7" authorId="0" shapeId="0">
       <text>
         <r>
@@ -966,7 +868,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="137">
   <si>
     <t>CommName</t>
   </si>
@@ -1094,9 +996,6 @@
     <t>* Values associate with commodities</t>
   </si>
   <si>
-    <t>&lt;more emission commodities here&gt;</t>
-  </si>
-  <si>
     <t>\I:Units</t>
   </si>
   <si>
@@ -1121,24 +1020,6 @@
     <t>*TechDesc</t>
   </si>
   <si>
-    <t>Attribute</t>
-  </si>
-  <si>
-    <t>Attribute Declaration Column</t>
-  </si>
-  <si>
-    <t>Base Year</t>
-  </si>
-  <si>
-    <t>TimeSlice</t>
-  </si>
-  <si>
-    <t>Time slices definition</t>
-  </si>
-  <si>
-    <t>Bound definition</t>
-  </si>
-  <si>
     <t>*Commodity Set Membership</t>
   </si>
   <si>
@@ -1163,9 +1044,6 @@
     <t>TimeSlice level of Process Activity</t>
   </si>
   <si>
-    <t>Typical structure for processes with several data years</t>
-  </si>
-  <si>
     <t>Fixed layout table</t>
   </si>
   <si>
@@ -1211,9 +1089,6 @@
     <t>COM_PROJ</t>
   </si>
   <si>
-    <t>IRE_PRICE</t>
-  </si>
-  <si>
     <t>*Unit</t>
   </si>
   <si>
@@ -1248,15 +1123,6 @@
   </si>
   <si>
     <t>Lifetime of Process</t>
-  </si>
-  <si>
-    <t>&lt;base year&gt;</t>
-  </si>
-  <si>
-    <t>&lt;more data years&gt;</t>
-  </si>
-  <si>
-    <t>Data Year</t>
   </si>
   <si>
     <t>FT-ELCCOA</t>
@@ -1418,12 +1284,12 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0000"/>
     <numFmt numFmtId="165" formatCode="\Te\x\t"/>
   </numFmts>
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1483,12 +1349,6 @@
     <font>
       <sz val="8"/>
       <color indexed="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <color indexed="8"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -1662,7 +1522,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="74">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1689,9 +1549,8 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -1714,7 +1573,7 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="4" applyFont="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="4" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="5"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="5" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="5" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1732,30 +1591,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" xfId="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" xfId="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="4" applyFont="1"/>
-    <xf numFmtId="1" fontId="4" fillId="8" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="4" applyFont="1"/>
     <xf numFmtId="2" fontId="4" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1788,10 +1624,10 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1803,10 +1639,10 @@
     <xf numFmtId="0" fontId="4" fillId="11" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -2322,201 +2158,201 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="B1:J13"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.85546875" customWidth="1"/>
-    <col min="2" max="2" width="15.5703125" customWidth="1"/>
-    <col min="3" max="3" width="19.42578125" customWidth="1"/>
-    <col min="4" max="4" width="14.140625" customWidth="1"/>
-    <col min="5" max="5" width="17.85546875" customWidth="1"/>
-    <col min="6" max="6" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.88671875" customWidth="1"/>
+    <col min="2" max="2" width="15.5546875" customWidth="1"/>
+    <col min="3" max="3" width="19.44140625" customWidth="1"/>
+    <col min="4" max="4" width="14.109375" customWidth="1"/>
+    <col min="5" max="5" width="17.88671875" customWidth="1"/>
+    <col min="6" max="6" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.44140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12" customWidth="1"/>
-    <col min="9" max="9" width="12.140625" customWidth="1"/>
-    <col min="10" max="10" width="10.140625" customWidth="1"/>
-    <col min="11" max="11" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.109375" customWidth="1"/>
+    <col min="10" max="10" width="10.109375" customWidth="1"/>
+    <col min="11" max="11" width="7.44140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="10.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:10" ht="21.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B1" s="45" t="s">
-        <v>66</v>
-      </c>
-      <c r="C1" s="45"/>
-    </row>
-    <row r="4" spans="2:10" ht="15" x14ac:dyDescent="0.2">
-      <c r="B4" s="25" t="s">
+      <c r="B1" s="32" t="s">
+        <v>58</v>
+      </c>
+      <c r="C1" s="32"/>
+    </row>
+    <row r="4" spans="2:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="B4" s="24" t="s">
         <v>34</v>
       </c>
-      <c r="C4" s="25"/>
-    </row>
-    <row r="6" spans="2:10" ht="18" x14ac:dyDescent="0.25">
-      <c r="B6" s="49" t="s">
-        <v>44</v>
-      </c>
-      <c r="C6" s="49"/>
-      <c r="D6" s="50"/>
-      <c r="E6" s="51"/>
-      <c r="F6" s="51"/>
-      <c r="G6" s="51"/>
-      <c r="H6" s="51"/>
-      <c r="I6" s="51"/>
-      <c r="J6" s="51"/>
-    </row>
-    <row r="7" spans="2:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="52" t="s">
+      <c r="C4" s="24"/>
+    </row>
+    <row r="6" spans="2:10" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="B6" s="35" t="s">
+        <v>43</v>
+      </c>
+      <c r="C6" s="35"/>
+      <c r="D6" s="36"/>
+      <c r="E6" s="37"/>
+      <c r="F6" s="37"/>
+      <c r="G6" s="37"/>
+      <c r="H6" s="37"/>
+      <c r="I6" s="37"/>
+      <c r="J6" s="37"/>
+    </row>
+    <row r="7" spans="2:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="38" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="52"/>
-      <c r="D7" s="51"/>
-      <c r="E7" s="51"/>
-      <c r="F7" s="51"/>
-      <c r="G7" s="51"/>
-      <c r="H7" s="51"/>
-      <c r="I7" s="51"/>
-      <c r="J7" s="51"/>
-    </row>
-    <row r="8" spans="2:10" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="53" t="s">
+      <c r="C7" s="38"/>
+      <c r="D7" s="37"/>
+      <c r="E7" s="37"/>
+      <c r="F7" s="37"/>
+      <c r="G7" s="37"/>
+      <c r="H7" s="37"/>
+      <c r="I7" s="37"/>
+      <c r="J7" s="37"/>
+    </row>
+    <row r="8" spans="2:10" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="54" t="s">
+      <c r="C8" s="40" t="s">
         <v>32</v>
       </c>
-      <c r="D8" s="53" t="s">
+      <c r="D8" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="E8" s="53" t="s">
+      <c r="E8" s="39" t="s">
         <v>3</v>
       </c>
-      <c r="F8" s="55" t="s">
+      <c r="F8" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="G8" s="55" t="s">
+      <c r="G8" s="41" t="s">
         <v>8</v>
       </c>
-      <c r="H8" s="55" t="s">
+      <c r="H8" s="41" t="s">
         <v>9</v>
       </c>
-      <c r="I8" s="55" t="s">
+      <c r="I8" s="41" t="s">
         <v>10</v>
       </c>
-      <c r="J8" s="55" t="s">
+      <c r="J8" s="41" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="2:10" ht="39" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="56" t="s">
-        <v>57</v>
-      </c>
-      <c r="C9" s="57" t="s">
+    <row r="9" spans="2:10" ht="40.200000000000003" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="42" t="s">
+        <v>50</v>
+      </c>
+      <c r="C9" s="43" t="s">
         <v>33</v>
       </c>
-      <c r="D9" s="56" t="s">
+      <c r="D9" s="42" t="s">
         <v>28</v>
       </c>
-      <c r="E9" s="56" t="s">
+      <c r="E9" s="42" t="s">
         <v>29</v>
       </c>
-      <c r="F9" s="56" t="s">
+      <c r="F9" s="42" t="s">
         <v>4</v>
       </c>
-      <c r="G9" s="56" t="s">
-        <v>60</v>
-      </c>
-      <c r="H9" s="56" t="s">
-        <v>61</v>
-      </c>
-      <c r="I9" s="56" t="s">
+      <c r="G9" s="42" t="s">
+        <v>53</v>
+      </c>
+      <c r="H9" s="42" t="s">
+        <v>54</v>
+      </c>
+      <c r="I9" s="42" t="s">
         <v>30</v>
       </c>
-      <c r="J9" s="56" t="s">
+      <c r="J9" s="42" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B10" s="65" t="s">
-        <v>132</v>
-      </c>
-      <c r="C10" s="72"/>
-      <c r="D10" s="65" t="s">
-        <v>133</v>
-      </c>
-      <c r="E10" s="65" t="s">
-        <v>134</v>
-      </c>
-      <c r="F10" s="65" t="s">
-        <v>135</v>
-      </c>
-      <c r="G10" s="65"/>
-      <c r="H10" s="65" t="s">
-        <v>136</v>
-      </c>
-      <c r="I10" s="65"/>
-      <c r="J10" s="65"/>
-    </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B11" s="65" t="s">
-        <v>137</v>
-      </c>
-      <c r="C11" s="72"/>
-      <c r="D11" s="65" t="s">
-        <v>100</v>
-      </c>
-      <c r="E11" s="65" t="s">
-        <v>138</v>
-      </c>
-      <c r="F11" s="65" t="s">
+    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B10" s="51" t="s">
+        <v>120</v>
+      </c>
+      <c r="C10" s="58"/>
+      <c r="D10" s="51" t="s">
+        <v>121</v>
+      </c>
+      <c r="E10" s="51" t="s">
+        <v>122</v>
+      </c>
+      <c r="F10" s="51" t="s">
+        <v>123</v>
+      </c>
+      <c r="G10" s="51"/>
+      <c r="H10" s="51" t="s">
+        <v>124</v>
+      </c>
+      <c r="I10" s="51"/>
+      <c r="J10" s="51"/>
+    </row>
+    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B11" s="51" t="s">
+        <v>125</v>
+      </c>
+      <c r="C11" s="58"/>
+      <c r="D11" s="51" t="s">
+        <v>88</v>
+      </c>
+      <c r="E11" s="51" t="s">
         <v>126</v>
       </c>
-      <c r="G11" s="65" t="s">
-        <v>129</v>
-      </c>
-      <c r="H11" s="65"/>
-      <c r="I11" s="65"/>
-      <c r="J11" s="65"/>
-    </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B12" s="65" t="s">
-        <v>137</v>
-      </c>
-      <c r="C12" s="72"/>
-      <c r="D12" s="65" t="s">
-        <v>108</v>
-      </c>
-      <c r="E12" s="65" t="s">
-        <v>139</v>
-      </c>
-      <c r="F12" s="65" t="s">
-        <v>126</v>
-      </c>
-      <c r="G12" s="65"/>
-      <c r="H12" s="65"/>
-      <c r="I12" s="65"/>
-      <c r="J12" s="65"/>
-    </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B13" s="65" t="s">
-        <v>137</v>
-      </c>
-      <c r="C13" s="72"/>
-      <c r="D13" s="65" t="s">
-        <v>111</v>
-      </c>
-      <c r="E13" s="65" t="s">
-        <v>140</v>
-      </c>
-      <c r="F13" s="65" t="s">
-        <v>126</v>
-      </c>
-      <c r="G13" s="65"/>
-      <c r="H13" s="65"/>
-      <c r="I13" s="65"/>
-      <c r="J13" s="65"/>
+      <c r="F11" s="51" t="s">
+        <v>114</v>
+      </c>
+      <c r="G11" s="51" t="s">
+        <v>117</v>
+      </c>
+      <c r="H11" s="51"/>
+      <c r="I11" s="51"/>
+      <c r="J11" s="51"/>
+    </row>
+    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B12" s="51" t="s">
+        <v>125</v>
+      </c>
+      <c r="C12" s="58"/>
+      <c r="D12" s="51" t="s">
+        <v>96</v>
+      </c>
+      <c r="E12" s="51" t="s">
+        <v>127</v>
+      </c>
+      <c r="F12" s="51" t="s">
+        <v>114</v>
+      </c>
+      <c r="G12" s="51"/>
+      <c r="H12" s="51"/>
+      <c r="I12" s="51"/>
+      <c r="J12" s="51"/>
+    </row>
+    <row r="13" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B13" s="51" t="s">
+        <v>125</v>
+      </c>
+      <c r="C13" s="58"/>
+      <c r="D13" s="51" t="s">
+        <v>99</v>
+      </c>
+      <c r="E13" s="51" t="s">
+        <v>128</v>
+      </c>
+      <c r="F13" s="51" t="s">
+        <v>114</v>
+      </c>
+      <c r="G13" s="51"/>
+      <c r="H13" s="51"/>
+      <c r="I13" s="51"/>
+      <c r="J13" s="51"/>
     </row>
   </sheetData>
   <phoneticPr fontId="0" type="noConversion"/>
@@ -2532,275 +2368,275 @@
   <dimension ref="A1:J15"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.140625" customWidth="1"/>
-    <col min="2" max="2" width="15.85546875" customWidth="1"/>
-    <col min="3" max="3" width="13.5703125" customWidth="1"/>
-    <col min="4" max="4" width="15.7109375" customWidth="1"/>
-    <col min="5" max="5" width="45.7109375" customWidth="1"/>
-    <col min="8" max="8" width="14.5703125" customWidth="1"/>
-    <col min="9" max="9" width="12.140625" customWidth="1"/>
+    <col min="1" max="1" width="3.109375" customWidth="1"/>
+    <col min="2" max="2" width="15.88671875" customWidth="1"/>
+    <col min="3" max="3" width="13.5546875" customWidth="1"/>
+    <col min="4" max="4" width="15.6640625" customWidth="1"/>
+    <col min="5" max="5" width="45.6640625" customWidth="1"/>
+    <col min="8" max="8" width="14.5546875" customWidth="1"/>
+    <col min="9" max="9" width="12.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="B1" s="45" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" ht="18" x14ac:dyDescent="0.25">
-      <c r="A2" s="14"/>
-    </row>
-    <row r="3" spans="1:10" ht="18" x14ac:dyDescent="0.25">
-      <c r="A3" s="14"/>
-      <c r="B3" s="25" t="s">
+    <row r="1" spans="1:10" ht="24.6" x14ac:dyDescent="0.4">
+      <c r="B1" s="32" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A2" s="13"/>
+    </row>
+    <row r="3" spans="1:10" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A3" s="13"/>
+      <c r="B3" s="24" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="13"/>
-      <c r="B5" s="49" t="s">
-        <v>45</v>
-      </c>
-      <c r="C5" s="58"/>
-      <c r="D5" s="58"/>
-      <c r="E5" s="58"/>
-      <c r="F5" s="58"/>
-      <c r="G5" s="58"/>
-      <c r="H5" s="58"/>
-      <c r="I5" s="58"/>
-      <c r="J5" s="58"/>
-    </row>
-    <row r="6" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="52" t="s">
+    <row r="5" spans="1:10" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="12"/>
+      <c r="B5" s="35" t="s">
+        <v>44</v>
+      </c>
+      <c r="C5" s="44"/>
+      <c r="D5" s="44"/>
+      <c r="E5" s="44"/>
+      <c r="F5" s="44"/>
+      <c r="G5" s="44"/>
+      <c r="H5" s="44"/>
+      <c r="I5" s="44"/>
+      <c r="J5" s="44"/>
+    </row>
+    <row r="6" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="38" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="52"/>
-      <c r="D6" s="58"/>
-      <c r="E6" s="58"/>
-      <c r="F6" s="58"/>
-      <c r="G6" s="58"/>
-      <c r="H6" s="58"/>
-      <c r="I6" s="58"/>
-      <c r="J6" s="58"/>
-    </row>
-    <row r="7" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="54" t="s">
+      <c r="C6" s="38"/>
+      <c r="D6" s="44"/>
+      <c r="E6" s="44"/>
+      <c r="F6" s="44"/>
+      <c r="G6" s="44"/>
+      <c r="H6" s="44"/>
+      <c r="I6" s="44"/>
+      <c r="J6" s="44"/>
+    </row>
+    <row r="7" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="40" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="54" t="s">
+      <c r="C7" s="40" t="s">
         <v>32</v>
       </c>
-      <c r="D7" s="54" t="s">
+      <c r="D7" s="40" t="s">
         <v>1</v>
       </c>
-      <c r="E7" s="54" t="s">
+      <c r="E7" s="40" t="s">
         <v>2</v>
       </c>
-      <c r="F7" s="54" t="s">
+      <c r="F7" s="40" t="s">
         <v>18</v>
       </c>
-      <c r="G7" s="54" t="s">
+      <c r="G7" s="40" t="s">
         <v>19</v>
       </c>
-      <c r="H7" s="54" t="s">
+      <c r="H7" s="40" t="s">
         <v>20</v>
       </c>
-      <c r="I7" s="54" t="s">
+      <c r="I7" s="40" t="s">
         <v>21</v>
       </c>
-      <c r="J7" s="54" t="s">
+      <c r="J7" s="40" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="39" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="57" t="s">
-        <v>58</v>
-      </c>
-      <c r="C8" s="57" t="s">
+    <row r="8" spans="1:10" ht="40.200000000000003" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="43" t="s">
+        <v>51</v>
+      </c>
+      <c r="C8" s="43" t="s">
         <v>33</v>
       </c>
-      <c r="D8" s="57" t="s">
+      <c r="D8" s="43" t="s">
         <v>23</v>
       </c>
-      <c r="E8" s="57" t="s">
+      <c r="E8" s="43" t="s">
         <v>24</v>
       </c>
-      <c r="F8" s="57" t="s">
+      <c r="F8" s="43" t="s">
         <v>25</v>
       </c>
-      <c r="G8" s="57" t="s">
+      <c r="G8" s="43" t="s">
         <v>26</v>
       </c>
-      <c r="H8" s="57" t="s">
-        <v>64</v>
-      </c>
-      <c r="I8" s="57" t="s">
-        <v>63</v>
-      </c>
-      <c r="J8" s="57" t="s">
+      <c r="H8" s="43" t="s">
+        <v>57</v>
+      </c>
+      <c r="I8" s="43" t="s">
+        <v>56</v>
+      </c>
+      <c r="J8" s="43" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B9" s="72" t="s">
-        <v>124</v>
-      </c>
-      <c r="C9" s="72"/>
-      <c r="D9" s="72" t="s">
-        <v>101</v>
-      </c>
-      <c r="E9" s="72" t="s">
-        <v>125</v>
-      </c>
-      <c r="F9" s="72" t="s">
-        <v>126</v>
-      </c>
-      <c r="G9" s="72" t="s">
-        <v>123</v>
-      </c>
-      <c r="H9" s="72"/>
-      <c r="I9" s="72"/>
-      <c r="J9" s="72"/>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B10" s="72" t="s">
-        <v>127</v>
-      </c>
-      <c r="C10" s="72"/>
-      <c r="D10" s="72" t="s">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B9" s="58" t="s">
+        <v>112</v>
+      </c>
+      <c r="C9" s="58"/>
+      <c r="D9" s="58" t="s">
+        <v>89</v>
+      </c>
+      <c r="E9" s="58" t="s">
+        <v>113</v>
+      </c>
+      <c r="F9" s="58" t="s">
+        <v>114</v>
+      </c>
+      <c r="G9" s="58" t="s">
+        <v>111</v>
+      </c>
+      <c r="H9" s="58"/>
+      <c r="I9" s="58"/>
+      <c r="J9" s="58"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B10" s="58" t="s">
+        <v>115</v>
+      </c>
+      <c r="C10" s="58"/>
+      <c r="D10" s="58" t="s">
+        <v>85</v>
+      </c>
+      <c r="E10" s="58" t="s">
+        <v>86</v>
+      </c>
+      <c r="F10" s="58" t="s">
+        <v>114</v>
+      </c>
+      <c r="G10" s="58" t="s">
+        <v>116</v>
+      </c>
+      <c r="H10" s="58" t="s">
+        <v>117</v>
+      </c>
+      <c r="I10" s="58"/>
+      <c r="J10" s="58"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B11" s="58" t="s">
+        <v>118</v>
+      </c>
+      <c r="C11" s="58"/>
+      <c r="D11" s="58" t="s">
+        <v>130</v>
+      </c>
+      <c r="E11" s="58" t="s">
+        <v>92</v>
+      </c>
+      <c r="F11" s="58" t="s">
+        <v>114</v>
+      </c>
+      <c r="G11" s="58" t="s">
+        <v>111</v>
+      </c>
+      <c r="H11" s="58"/>
+      <c r="I11" s="58"/>
+      <c r="J11" s="58"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B12" s="58" t="s">
+        <v>119</v>
+      </c>
+      <c r="C12" s="58"/>
+      <c r="D12" s="58" t="s">
+        <v>94</v>
+      </c>
+      <c r="E12" s="58" t="s">
+        <v>95</v>
+      </c>
+      <c r="F12" s="58" t="s">
+        <v>114</v>
+      </c>
+      <c r="G12" s="58" t="s">
+        <v>111</v>
+      </c>
+      <c r="H12" s="58"/>
+      <c r="I12" s="58"/>
+      <c r="J12" s="58"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B13" s="58" t="s">
+        <v>119</v>
+      </c>
+      <c r="C13" s="58"/>
+      <c r="D13" s="58" t="s">
         <v>97</v>
       </c>
-      <c r="E10" s="72" t="s">
+      <c r="E13" s="58" t="s">
         <v>98</v>
       </c>
-      <c r="F10" s="72" t="s">
-        <v>126</v>
-      </c>
-      <c r="G10" s="72" t="s">
-        <v>128</v>
-      </c>
-      <c r="H10" s="72" t="s">
-        <v>129</v>
-      </c>
-      <c r="I10" s="72"/>
-      <c r="J10" s="72"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B11" s="72" t="s">
-        <v>130</v>
-      </c>
-      <c r="C11" s="72"/>
-      <c r="D11" s="72" t="s">
-        <v>142</v>
-      </c>
-      <c r="E11" s="72" t="s">
-        <v>104</v>
-      </c>
-      <c r="F11" s="72" t="s">
-        <v>126</v>
-      </c>
-      <c r="G11" s="72" t="s">
-        <v>123</v>
-      </c>
-      <c r="H11" s="72"/>
-      <c r="I11" s="72"/>
-      <c r="J11" s="72"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B12" s="72" t="s">
-        <v>131</v>
-      </c>
-      <c r="C12" s="72"/>
-      <c r="D12" s="72" t="s">
-        <v>106</v>
-      </c>
-      <c r="E12" s="72" t="s">
-        <v>107</v>
-      </c>
-      <c r="F12" s="72" t="s">
-        <v>126</v>
-      </c>
-      <c r="G12" s="72" t="s">
-        <v>123</v>
-      </c>
-      <c r="H12" s="72"/>
-      <c r="I12" s="72"/>
-      <c r="J12" s="72"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B13" s="72" t="s">
-        <v>131</v>
-      </c>
-      <c r="C13" s="72"/>
-      <c r="D13" s="72" t="s">
-        <v>109</v>
-      </c>
-      <c r="E13" s="72" t="s">
-        <v>110</v>
-      </c>
-      <c r="F13" s="72" t="s">
-        <v>126</v>
-      </c>
-      <c r="G13" s="72" t="s">
-        <v>123</v>
-      </c>
-      <c r="H13" s="72"/>
-      <c r="I13" s="72"/>
-      <c r="J13" s="72"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B14" s="72" t="s">
-        <v>127</v>
-      </c>
-      <c r="C14" s="72"/>
-      <c r="D14" s="72" t="str">
+      <c r="F13" s="58" t="s">
+        <v>114</v>
+      </c>
+      <c r="G13" s="58" t="s">
+        <v>111</v>
+      </c>
+      <c r="H13" s="58"/>
+      <c r="I13" s="58"/>
+      <c r="J13" s="58"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B14" s="58" t="s">
+        <v>115</v>
+      </c>
+      <c r="C14" s="58"/>
+      <c r="D14" s="58" t="str">
         <f>ProcessCharac!B17</f>
         <v>FT-ELCNGA</v>
       </c>
-      <c r="E14" s="72" t="str">
+      <c r="E14" s="58" t="str">
         <f>ProcessCharac!C17</f>
         <v>Fuel Technology Natural Gas ELC</v>
       </c>
-      <c r="F14" s="72" t="s">
-        <v>126</v>
-      </c>
-      <c r="G14" s="72" t="s">
-        <v>128</v>
-      </c>
-      <c r="H14" s="72" t="s">
-        <v>129</v>
-      </c>
-      <c r="I14" s="72"/>
-      <c r="J14" s="72"/>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B15" s="72" t="s">
-        <v>127</v>
-      </c>
-      <c r="C15" s="72"/>
-      <c r="D15" s="72" t="str">
+      <c r="F14" s="58" t="s">
+        <v>114</v>
+      </c>
+      <c r="G14" s="58" t="s">
+        <v>116</v>
+      </c>
+      <c r="H14" s="58" t="s">
+        <v>117</v>
+      </c>
+      <c r="I14" s="58"/>
+      <c r="J14" s="58"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B15" s="58" t="s">
+        <v>115</v>
+      </c>
+      <c r="C15" s="58"/>
+      <c r="D15" s="58" t="str">
         <f>ProcessCharac!B18</f>
         <v>FT-ELCWIN</v>
       </c>
-      <c r="E15" s="72" t="str">
+      <c r="E15" s="58" t="str">
         <f>ProcessCharac!C18</f>
         <v>Fuel Technology Wind ELC</v>
       </c>
-      <c r="F15" s="72" t="s">
-        <v>126</v>
-      </c>
-      <c r="G15" s="72" t="s">
-        <v>128</v>
-      </c>
-      <c r="H15" s="72" t="s">
-        <v>129</v>
-      </c>
-      <c r="I15" s="72"/>
-      <c r="J15" s="72"/>
+      <c r="F15" s="58" t="s">
+        <v>114</v>
+      </c>
+      <c r="G15" s="58" t="s">
+        <v>116</v>
+      </c>
+      <c r="H15" s="58" t="s">
+        <v>117</v>
+      </c>
+      <c r="I15" s="58"/>
+      <c r="J15" s="58"/>
     </row>
   </sheetData>
   <phoneticPr fontId="0" type="noConversion"/>
@@ -2816,42 +2652,42 @@
   <dimension ref="B1:V30"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="O17" sqref="O17"/>
+      <selection activeCell="F37" sqref="F37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.85546875" customWidth="1"/>
-    <col min="2" max="2" width="15.5703125" customWidth="1"/>
-    <col min="3" max="3" width="43.42578125" customWidth="1"/>
-    <col min="4" max="9" width="11.7109375" customWidth="1"/>
-    <col min="10" max="10" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.140625" customWidth="1"/>
-    <col min="12" max="12" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="15" max="17" width="13.5703125" customWidth="1"/>
-    <col min="18" max="18" width="18.7109375" customWidth="1"/>
-    <col min="19" max="19" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="13.42578125" customWidth="1"/>
-    <col min="21" max="21" width="12.85546875" customWidth="1"/>
-    <col min="22" max="22" width="13.28515625" customWidth="1"/>
-    <col min="23" max="24" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.88671875" customWidth="1"/>
+    <col min="2" max="2" width="15.5546875" customWidth="1"/>
+    <col min="3" max="3" width="43.44140625" customWidth="1"/>
+    <col min="4" max="9" width="11.6640625" customWidth="1"/>
+    <col min="10" max="10" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.109375" customWidth="1"/>
+    <col min="12" max="12" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="17" width="13.5546875" customWidth="1"/>
+    <col min="18" max="18" width="18.6640625" customWidth="1"/>
+    <col min="19" max="19" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="13.44140625" customWidth="1"/>
+    <col min="21" max="21" width="12.88671875" customWidth="1"/>
+    <col min="22" max="22" width="13.33203125" customWidth="1"/>
+    <col min="23" max="24" width="10.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:22" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="B1" s="45" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="3" spans="2:22" ht="18" x14ac:dyDescent="0.25">
-      <c r="B3" s="14" t="s">
+    <row r="1" spans="2:22" ht="24.6" x14ac:dyDescent="0.4">
+      <c r="B1" s="32" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="3" spans="2:22" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="B3" s="13" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="5" spans="2:22" ht="15" x14ac:dyDescent="0.2">
-      <c r="B5" s="25" t="s">
-        <v>62</v>
+    <row r="5" spans="2:22" ht="15" x14ac:dyDescent="0.25">
+      <c r="B5" s="24" t="s">
+        <v>55</v>
       </c>
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
@@ -2865,7 +2701,7 @@
       <c r="Q5" s="6"/>
       <c r="R5" s="6"/>
     </row>
-    <row r="6" spans="2:22" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B6" s="9"/>
       <c r="C6" s="2"/>
       <c r="E6" s="4"/>
@@ -2881,586 +2717,586 @@
       <c r="R6" s="6"/>
       <c r="S6" s="6"/>
     </row>
-    <row r="7" spans="2:22" x14ac:dyDescent="0.2">
-      <c r="F7" s="30"/>
-      <c r="H7" s="30" t="s">
+    <row r="7" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="F7" s="29"/>
+      <c r="H7" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="I7" s="30"/>
-      <c r="J7" s="31"/>
-      <c r="K7" s="27"/>
-      <c r="L7" s="27"/>
-      <c r="M7" s="32"/>
-      <c r="N7" s="26"/>
-      <c r="O7" s="28"/>
-      <c r="P7" s="29"/>
-      <c r="Q7" s="26"/>
-      <c r="R7" s="26"/>
-      <c r="S7" s="28"/>
-    </row>
-    <row r="8" spans="2:22" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="60" t="s">
+      <c r="I7" s="29"/>
+      <c r="J7" s="30"/>
+      <c r="K7" s="26"/>
+      <c r="L7" s="26"/>
+      <c r="M7" s="31"/>
+      <c r="N7" s="25"/>
+      <c r="O7" s="27"/>
+      <c r="P7" s="28"/>
+      <c r="Q7" s="25"/>
+      <c r="R7" s="25"/>
+      <c r="S7" s="27"/>
+    </row>
+    <row r="8" spans="2:22" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="46" t="s">
         <v>1</v>
       </c>
-      <c r="C8" s="61" t="s">
-        <v>50</v>
-      </c>
-      <c r="D8" s="60" t="s">
+      <c r="C8" s="47" t="s">
+        <v>49</v>
+      </c>
+      <c r="D8" s="46" t="s">
         <v>5</v>
       </c>
-      <c r="E8" s="60" t="s">
+      <c r="E8" s="46" t="s">
         <v>6</v>
       </c>
-      <c r="F8" s="60" t="s">
+      <c r="F8" s="46" t="s">
+        <v>61</v>
+      </c>
+      <c r="G8" s="46" t="s">
+        <v>76</v>
+      </c>
+      <c r="H8" s="46" t="s">
+        <v>60</v>
+      </c>
+      <c r="I8" s="34" t="s">
+        <v>15</v>
+      </c>
+      <c r="J8" s="34" t="s">
+        <v>71</v>
+      </c>
+      <c r="K8" s="34" t="s">
+        <v>62</v>
+      </c>
+      <c r="L8" s="34" t="s">
+        <v>70</v>
+      </c>
+      <c r="M8" s="34" t="s">
+        <v>66</v>
+      </c>
+      <c r="N8" s="34" t="s">
+        <v>67</v>
+      </c>
+      <c r="O8" s="34" t="s">
+        <v>83</v>
+      </c>
+      <c r="P8" s="34" t="s">
+        <v>68</v>
+      </c>
+      <c r="Q8" s="48" t="s">
+        <v>65</v>
+      </c>
+      <c r="R8" s="34" t="s">
         <v>69</v>
       </c>
-      <c r="G8" s="60" t="s">
+      <c r="S8" s="54" t="s">
+        <v>102</v>
+      </c>
+      <c r="T8" s="54" t="s">
+        <v>103</v>
+      </c>
+      <c r="U8" s="54" t="s">
+        <v>104</v>
+      </c>
+      <c r="V8" s="54" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="9" spans="2:22" ht="42.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="45" t="s">
+        <v>52</v>
+      </c>
+      <c r="C9" s="45" t="s">
+        <v>24</v>
+      </c>
+      <c r="D9" s="45" t="s">
+        <v>37</v>
+      </c>
+      <c r="E9" s="45" t="s">
+        <v>38</v>
+      </c>
+      <c r="F9" s="45" t="s">
+        <v>78</v>
+      </c>
+      <c r="G9" s="45" t="s">
+        <v>76</v>
+      </c>
+      <c r="H9" s="45" t="s">
+        <v>77</v>
+      </c>
+      <c r="I9" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="J9" s="45" t="s">
+        <v>79</v>
+      </c>
+      <c r="K9" s="45" t="s">
+        <v>81</v>
+      </c>
+      <c r="L9" s="45" t="s">
+        <v>46</v>
+      </c>
+      <c r="M9" s="45" t="s">
+        <v>45</v>
+      </c>
+      <c r="N9" s="45" t="s">
+        <v>82</v>
+      </c>
+      <c r="O9" s="45" t="s">
+        <v>84</v>
+      </c>
+      <c r="P9" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q9" s="45" t="s">
+        <v>74</v>
+      </c>
+      <c r="R9" s="45" t="s">
+        <v>80</v>
+      </c>
+      <c r="S9" s="55" t="s">
+        <v>106</v>
+      </c>
+      <c r="T9" s="55" t="s">
+        <v>107</v>
+      </c>
+      <c r="U9" s="55" t="s">
+        <v>108</v>
+      </c>
+      <c r="V9" s="55" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="10" spans="2:22" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B10" s="49" t="s">
+        <v>73</v>
+      </c>
+      <c r="C10" s="50"/>
+      <c r="D10" s="50"/>
+      <c r="E10" s="50"/>
+      <c r="F10" s="50"/>
+      <c r="G10" s="49"/>
+      <c r="H10" s="49"/>
+      <c r="I10" s="49"/>
+      <c r="J10" s="49"/>
+      <c r="K10" s="49"/>
+      <c r="L10" s="49"/>
+      <c r="M10" s="49"/>
+      <c r="N10" s="49"/>
+      <c r="O10" s="50"/>
+      <c r="P10" s="49"/>
+      <c r="Q10" s="50"/>
+      <c r="R10" s="50"/>
+      <c r="S10" s="56" t="s">
+        <v>110</v>
+      </c>
+      <c r="T10" s="56" t="s">
+        <v>111</v>
+      </c>
+      <c r="U10" s="57"/>
+      <c r="V10" s="57"/>
+    </row>
+    <row r="11" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B11" s="18" t="s">
         <v>85</v>
       </c>
-      <c r="H8" s="60" t="s">
-        <v>68</v>
-      </c>
-      <c r="I8" s="48" t="s">
-        <v>15</v>
-      </c>
-      <c r="J8" s="48" t="s">
-        <v>79</v>
-      </c>
-      <c r="K8" s="48" t="s">
-        <v>70</v>
-      </c>
-      <c r="L8" s="48" t="s">
-        <v>78</v>
-      </c>
-      <c r="M8" s="48" t="s">
-        <v>74</v>
-      </c>
-      <c r="N8" s="48" t="s">
+      <c r="C11" s="18" t="s">
+        <v>86</v>
+      </c>
+      <c r="D11" s="18" t="s">
+        <v>87</v>
+      </c>
+      <c r="E11" s="18" t="s">
+        <v>88</v>
+      </c>
+      <c r="F11" s="18"/>
+      <c r="G11" s="18"/>
+      <c r="H11" s="18"/>
+      <c r="I11" s="18">
+        <v>1</v>
+      </c>
+      <c r="J11" s="18"/>
+      <c r="K11" s="18"/>
+      <c r="L11" s="51"/>
+      <c r="M11" s="51"/>
+      <c r="N11" s="18"/>
+      <c r="O11" s="18"/>
+      <c r="P11" s="51"/>
+      <c r="Q11" s="18"/>
+      <c r="R11" s="18"/>
+      <c r="S11" s="51"/>
+      <c r="T11" s="51"/>
+      <c r="U11" s="51"/>
+      <c r="V11" s="51"/>
+    </row>
+    <row r="12" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B12" s="18" t="s">
+        <v>89</v>
+      </c>
+      <c r="C12" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="D12" s="18" t="s">
+        <v>88</v>
+      </c>
+      <c r="E12" s="18" t="s">
+        <v>91</v>
+      </c>
+      <c r="F12" s="18"/>
+      <c r="G12" s="18">
+        <v>2012</v>
+      </c>
+      <c r="H12" s="18" t="s">
+        <v>100</v>
+      </c>
+      <c r="I12" s="18">
+        <v>0.437</v>
+      </c>
+      <c r="J12" s="18"/>
+      <c r="K12" s="33"/>
+      <c r="L12" s="51">
+        <v>2.145E-2</v>
+      </c>
+      <c r="M12" s="51">
+        <v>0.93089999999999995</v>
+      </c>
+      <c r="N12" s="18"/>
+      <c r="O12" s="18">
+        <v>40</v>
+      </c>
+      <c r="P12" s="51">
+        <v>3.1536000000000002E-2</v>
+      </c>
+      <c r="Q12" s="18"/>
+      <c r="R12" s="33"/>
+      <c r="S12" s="51">
+        <v>0.85099999999999998</v>
+      </c>
+      <c r="T12" s="51">
+        <v>108.2</v>
+      </c>
+      <c r="U12" s="51">
+        <v>1</v>
+      </c>
+      <c r="V12" s="51"/>
+    </row>
+    <row r="13" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B13" s="18" t="s">
+        <v>130</v>
+      </c>
+      <c r="C13" s="18" t="s">
+        <v>92</v>
+      </c>
+      <c r="D13" s="18" t="s">
+        <v>88</v>
+      </c>
+      <c r="E13" s="18" t="s">
+        <v>91</v>
+      </c>
+      <c r="F13" s="18"/>
+      <c r="G13" s="18">
+        <v>2012</v>
+      </c>
+      <c r="H13" s="18" t="s">
+        <v>100</v>
+      </c>
+      <c r="I13" s="18">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="J13" s="18"/>
+      <c r="K13" s="33"/>
+      <c r="L13" s="52">
+        <v>0.1</v>
+      </c>
+      <c r="M13" s="52">
+        <v>0.6</v>
+      </c>
+      <c r="N13" s="18"/>
+      <c r="O13" s="18">
+        <v>35</v>
+      </c>
+      <c r="P13" s="51">
+        <v>3.1536000000000002E-2</v>
+      </c>
+      <c r="Q13" s="18"/>
+      <c r="R13" s="33"/>
+      <c r="S13" s="51">
+        <v>0.86</v>
+      </c>
+      <c r="T13" s="51">
+        <v>90000</v>
+      </c>
+      <c r="U13" s="51">
+        <v>1</v>
+      </c>
+      <c r="V13" s="51">
+        <v>2.1</v>
+      </c>
+    </row>
+    <row r="14" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B14" s="18"/>
+      <c r="C14" s="18"/>
+      <c r="D14" s="18"/>
+      <c r="E14" s="18" t="s">
+        <v>93</v>
+      </c>
+      <c r="F14" s="18"/>
+      <c r="G14" s="18"/>
+      <c r="H14" s="18"/>
+      <c r="I14" s="18"/>
+      <c r="J14" s="18"/>
+      <c r="K14" s="33"/>
+      <c r="L14" s="51"/>
+      <c r="M14" s="51"/>
+      <c r="N14" s="18"/>
+      <c r="O14" s="18"/>
+      <c r="P14" s="51"/>
+      <c r="Q14" s="18"/>
+      <c r="R14" s="33"/>
+      <c r="S14" s="51"/>
+      <c r="T14" s="51"/>
+      <c r="U14" s="51"/>
+      <c r="V14" s="51"/>
+    </row>
+    <row r="15" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B15" s="18" t="s">
+        <v>94</v>
+      </c>
+      <c r="C15" s="18" t="s">
+        <v>95</v>
+      </c>
+      <c r="D15" s="18" t="s">
+        <v>96</v>
+      </c>
+      <c r="E15" s="18" t="s">
+        <v>91</v>
+      </c>
+      <c r="F15" s="18"/>
+      <c r="G15" s="18">
+        <v>2012</v>
+      </c>
+      <c r="H15" s="18" t="s">
+        <v>101</v>
+      </c>
+      <c r="I15" s="18">
+        <v>0.39</v>
+      </c>
+      <c r="J15" s="18"/>
+      <c r="K15" s="33"/>
+      <c r="L15" s="51">
+        <v>0.02</v>
+      </c>
+      <c r="M15" s="51">
+        <v>1.25</v>
+      </c>
+      <c r="N15" s="18"/>
+      <c r="O15" s="18">
+        <v>25</v>
+      </c>
+      <c r="P15" s="51">
+        <v>3.1536000000000002E-2</v>
+      </c>
+      <c r="Q15" s="18"/>
+      <c r="R15" s="33"/>
+      <c r="S15" s="52">
+        <v>0.92346153799999997</v>
+      </c>
+      <c r="T15" s="51">
+        <v>100</v>
+      </c>
+      <c r="U15" s="51">
+        <v>1</v>
+      </c>
+      <c r="V15" s="51"/>
+    </row>
+    <row r="16" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B16" s="18" t="s">
+        <v>97</v>
+      </c>
+      <c r="C16" s="18" t="s">
+        <v>98</v>
+      </c>
+      <c r="D16" s="18" t="s">
+        <v>99</v>
+      </c>
+      <c r="E16" s="18" t="s">
+        <v>91</v>
+      </c>
+      <c r="F16" s="18"/>
+      <c r="G16" s="18">
+        <v>2012</v>
+      </c>
+      <c r="H16" s="18" t="s">
+        <v>101</v>
+      </c>
+      <c r="I16" s="18">
+        <v>1</v>
+      </c>
+      <c r="J16" s="33"/>
+      <c r="K16" s="33"/>
+      <c r="L16" s="53">
+        <v>2.5599999999999998E-2</v>
+      </c>
+      <c r="M16" s="53">
+        <v>0.77777777777777779</v>
+      </c>
+      <c r="N16" s="33"/>
+      <c r="O16" s="33">
+        <v>25</v>
+      </c>
+      <c r="P16" s="51">
+        <v>3.1536000000000002E-2</v>
+      </c>
+      <c r="Q16" s="33"/>
+      <c r="R16" s="33"/>
+      <c r="S16" s="51">
+        <v>0.37</v>
+      </c>
+      <c r="T16" s="51">
+        <v>100</v>
+      </c>
+      <c r="U16" s="51">
+        <v>1</v>
+      </c>
+      <c r="V16" s="51"/>
+    </row>
+    <row r="17" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B17" s="18" t="s">
+        <v>131</v>
+      </c>
+      <c r="C17" s="18" t="s">
+        <v>132</v>
+      </c>
+      <c r="D17" s="18" t="s">
+        <v>133</v>
+      </c>
+      <c r="E17" s="18" t="s">
+        <v>96</v>
+      </c>
+      <c r="F17" s="18"/>
+      <c r="G17" s="18"/>
+      <c r="H17" s="18"/>
+      <c r="I17" s="18">
+        <v>1</v>
+      </c>
+      <c r="J17" s="18"/>
+      <c r="K17" s="18"/>
+      <c r="L17" s="51"/>
+      <c r="M17" s="18"/>
+      <c r="N17" s="18"/>
+      <c r="O17" s="51"/>
+      <c r="P17" s="18"/>
+      <c r="Q17" s="18"/>
+      <c r="R17" s="51"/>
+      <c r="S17" s="18"/>
+      <c r="T17" s="18"/>
+      <c r="U17" s="51"/>
+      <c r="V17" s="51"/>
+    </row>
+    <row r="18" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B18" s="18" t="s">
+        <v>134</v>
+      </c>
+      <c r="C18" s="18" t="s">
+        <v>135</v>
+      </c>
+      <c r="D18" s="18" t="s">
+        <v>136</v>
+      </c>
+      <c r="E18" s="18" t="s">
+        <v>99</v>
+      </c>
+      <c r="F18" s="18"/>
+      <c r="G18" s="18"/>
+      <c r="H18" s="18"/>
+      <c r="I18" s="18">
+        <v>1</v>
+      </c>
+      <c r="J18" s="18"/>
+      <c r="K18" s="18"/>
+      <c r="L18" s="51"/>
+      <c r="M18" s="18"/>
+      <c r="N18" s="18"/>
+      <c r="O18" s="51"/>
+      <c r="P18" s="18"/>
+      <c r="Q18" s="18"/>
+      <c r="R18" s="51"/>
+      <c r="S18" s="18"/>
+      <c r="T18" s="18"/>
+      <c r="U18" s="51"/>
+      <c r="V18" s="51"/>
+    </row>
+    <row r="19" spans="2:22" ht="24.6" x14ac:dyDescent="0.4">
+      <c r="B19" s="32" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="22" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B22" s="22" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="23" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B23" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="C23" s="21" t="s">
         <v>75</v>
       </c>
-      <c r="O8" s="48" t="s">
-        <v>92</v>
-      </c>
-      <c r="P8" s="48" t="s">
-        <v>76</v>
-      </c>
-      <c r="Q8" s="62" t="s">
+      <c r="D23" s="21" t="s">
         <v>73</v>
       </c>
-      <c r="R8" s="48" t="s">
-        <v>77</v>
-      </c>
-      <c r="S8" s="68" t="s">
-        <v>114</v>
-      </c>
-      <c r="T8" s="68" t="s">
-        <v>115</v>
-      </c>
-      <c r="U8" s="68" t="s">
-        <v>116</v>
-      </c>
-      <c r="V8" s="68" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="9" spans="2:22" ht="42.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="59" t="s">
-        <v>59</v>
-      </c>
-      <c r="C9" s="59" t="s">
-        <v>24</v>
-      </c>
-      <c r="D9" s="59" t="s">
-        <v>37</v>
-      </c>
-      <c r="E9" s="59" t="s">
-        <v>38</v>
-      </c>
-      <c r="F9" s="59" t="s">
-        <v>87</v>
-      </c>
-      <c r="G9" s="59" t="s">
-        <v>85</v>
-      </c>
-      <c r="H9" s="59" t="s">
-        <v>86</v>
-      </c>
-      <c r="I9" s="59" t="s">
-        <v>39</v>
-      </c>
-      <c r="J9" s="59" t="s">
-        <v>88</v>
-      </c>
-      <c r="K9" s="59" t="s">
-        <v>90</v>
-      </c>
-      <c r="L9" s="59" t="s">
+      <c r="E23" s="21" t="s">
+        <v>72</v>
+      </c>
+      <c r="F23" s="1"/>
+    </row>
+    <row r="24" spans="2:22" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B24" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="M9" s="59" t="s">
-        <v>46</v>
-      </c>
-      <c r="N9" s="59" t="s">
-        <v>91</v>
-      </c>
-      <c r="O9" s="59" t="s">
-        <v>93</v>
-      </c>
-      <c r="P9" s="59" t="s">
-        <v>40</v>
-      </c>
-      <c r="Q9" s="59" t="s">
-        <v>83</v>
-      </c>
-      <c r="R9" s="59" t="s">
-        <v>89</v>
-      </c>
-      <c r="S9" s="69" t="s">
-        <v>118</v>
-      </c>
-      <c r="T9" s="69" t="s">
-        <v>119</v>
-      </c>
-      <c r="U9" s="69" t="s">
-        <v>120</v>
-      </c>
-      <c r="V9" s="69" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="10" spans="2:22" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="63" t="s">
-        <v>82</v>
-      </c>
-      <c r="C10" s="64"/>
-      <c r="D10" s="64"/>
-      <c r="E10" s="64"/>
-      <c r="F10" s="64"/>
-      <c r="G10" s="63"/>
-      <c r="H10" s="63"/>
-      <c r="I10" s="63"/>
-      <c r="J10" s="63"/>
-      <c r="K10" s="63"/>
-      <c r="L10" s="63"/>
-      <c r="M10" s="63"/>
-      <c r="N10" s="63"/>
-      <c r="O10" s="64"/>
-      <c r="P10" s="63"/>
-      <c r="Q10" s="64"/>
-      <c r="R10" s="64"/>
-      <c r="S10" s="70" t="s">
-        <v>122</v>
-      </c>
-      <c r="T10" s="70" t="s">
-        <v>123</v>
-      </c>
-      <c r="U10" s="71"/>
-      <c r="V10" s="71"/>
-    </row>
-    <row r="11" spans="2:22" x14ac:dyDescent="0.2">
-      <c r="B11" s="19" t="s">
-        <v>97</v>
-      </c>
-      <c r="C11" s="19" t="s">
-        <v>98</v>
-      </c>
-      <c r="D11" s="19" t="s">
-        <v>99</v>
-      </c>
-      <c r="E11" s="19" t="s">
-        <v>100</v>
-      </c>
-      <c r="F11" s="19"/>
-      <c r="G11" s="19"/>
-      <c r="H11" s="19"/>
-      <c r="I11" s="19">
-        <v>1</v>
-      </c>
-      <c r="J11" s="19"/>
-      <c r="K11" s="19"/>
-      <c r="L11" s="65"/>
-      <c r="M11" s="65"/>
-      <c r="N11" s="19"/>
-      <c r="O11" s="19"/>
-      <c r="P11" s="65"/>
-      <c r="Q11" s="19"/>
-      <c r="R11" s="19"/>
-      <c r="S11" s="65"/>
-      <c r="T11" s="65"/>
-      <c r="U11" s="65"/>
-      <c r="V11" s="65"/>
-    </row>
-    <row r="12" spans="2:22" x14ac:dyDescent="0.2">
-      <c r="B12" s="19" t="s">
-        <v>101</v>
-      </c>
-      <c r="C12" s="19" t="s">
-        <v>102</v>
-      </c>
-      <c r="D12" s="19" t="s">
-        <v>100</v>
-      </c>
-      <c r="E12" s="19" t="s">
-        <v>103</v>
-      </c>
-      <c r="F12" s="19"/>
-      <c r="G12" s="19">
-        <v>2012</v>
-      </c>
-      <c r="H12" s="19" t="s">
-        <v>112</v>
-      </c>
-      <c r="I12" s="19">
-        <v>0.437</v>
-      </c>
-      <c r="J12" s="19"/>
-      <c r="K12" s="47"/>
-      <c r="L12" s="65">
-        <v>2.145E-2</v>
-      </c>
-      <c r="M12" s="65">
-        <v>0.93089999999999995</v>
-      </c>
-      <c r="N12" s="19"/>
-      <c r="O12" s="19">
-        <v>40</v>
-      </c>
-      <c r="P12" s="65">
-        <v>3.1536000000000002E-2</v>
-      </c>
-      <c r="Q12" s="19"/>
-      <c r="R12" s="47"/>
-      <c r="S12" s="65">
-        <v>0.85099999999999998</v>
-      </c>
-      <c r="T12" s="65">
-        <v>108.2</v>
-      </c>
-      <c r="U12" s="65">
-        <v>1</v>
-      </c>
-      <c r="V12" s="65"/>
-    </row>
-    <row r="13" spans="2:22" x14ac:dyDescent="0.2">
-      <c r="B13" s="19" t="s">
-        <v>142</v>
-      </c>
-      <c r="C13" s="19" t="s">
-        <v>104</v>
-      </c>
-      <c r="D13" s="19" t="s">
-        <v>100</v>
-      </c>
-      <c r="E13" s="19" t="s">
-        <v>103</v>
-      </c>
-      <c r="F13" s="19"/>
-      <c r="G13" s="19">
-        <v>2012</v>
-      </c>
-      <c r="H13" s="19" t="s">
-        <v>112</v>
-      </c>
-      <c r="I13" s="19">
-        <v>0.28000000000000003</v>
-      </c>
-      <c r="J13" s="19"/>
-      <c r="K13" s="47"/>
-      <c r="L13" s="66">
-        <v>0.1</v>
-      </c>
-      <c r="M13" s="66">
-        <v>0.6</v>
-      </c>
-      <c r="N13" s="19"/>
-      <c r="O13" s="19">
-        <v>35</v>
-      </c>
-      <c r="P13" s="65">
-        <v>3.1536000000000002E-2</v>
-      </c>
-      <c r="Q13" s="19"/>
-      <c r="R13" s="47"/>
-      <c r="S13" s="65">
-        <v>0.86</v>
-      </c>
-      <c r="T13" s="65">
-        <v>90000</v>
-      </c>
-      <c r="U13" s="65">
-        <v>1</v>
-      </c>
-      <c r="V13" s="65">
-        <v>2.1</v>
-      </c>
-    </row>
-    <row r="14" spans="2:22" x14ac:dyDescent="0.2">
-      <c r="B14" s="19"/>
-      <c r="C14" s="19"/>
-      <c r="D14" s="19"/>
-      <c r="E14" s="19" t="s">
-        <v>105</v>
-      </c>
-      <c r="F14" s="19"/>
-      <c r="G14" s="19"/>
-      <c r="H14" s="19"/>
-      <c r="I14" s="19"/>
-      <c r="J14" s="19"/>
-      <c r="K14" s="47"/>
-      <c r="L14" s="65"/>
-      <c r="M14" s="65"/>
-      <c r="N14" s="19"/>
-      <c r="O14" s="19"/>
-      <c r="P14" s="65"/>
-      <c r="Q14" s="19"/>
-      <c r="R14" s="47"/>
-      <c r="S14" s="65"/>
-      <c r="T14" s="65"/>
-      <c r="U14" s="65"/>
-      <c r="V14" s="65"/>
-    </row>
-    <row r="15" spans="2:22" x14ac:dyDescent="0.2">
-      <c r="B15" s="19" t="s">
-        <v>106</v>
-      </c>
-      <c r="C15" s="19" t="s">
-        <v>107</v>
-      </c>
-      <c r="D15" s="19" t="s">
-        <v>108</v>
-      </c>
-      <c r="E15" s="19" t="s">
-        <v>103</v>
-      </c>
-      <c r="F15" s="19"/>
-      <c r="G15" s="19">
-        <v>2012</v>
-      </c>
-      <c r="H15" s="19" t="s">
-        <v>113</v>
-      </c>
-      <c r="I15" s="19">
-        <v>0.39</v>
-      </c>
-      <c r="J15" s="19"/>
-      <c r="K15" s="47"/>
-      <c r="L15" s="65">
-        <v>0.02</v>
-      </c>
-      <c r="M15" s="65">
-        <v>1.25</v>
-      </c>
-      <c r="N15" s="19"/>
-      <c r="O15" s="19">
-        <v>25</v>
-      </c>
-      <c r="P15" s="65">
-        <v>3.1536000000000002E-2</v>
-      </c>
-      <c r="Q15" s="19"/>
-      <c r="R15" s="47"/>
-      <c r="S15" s="66">
-        <v>0.92346153799999997</v>
-      </c>
-      <c r="T15" s="65">
-        <v>100</v>
-      </c>
-      <c r="U15" s="65">
-        <v>1</v>
-      </c>
-      <c r="V15" s="65"/>
-    </row>
-    <row r="16" spans="2:22" x14ac:dyDescent="0.2">
-      <c r="B16" s="19" t="s">
-        <v>109</v>
-      </c>
-      <c r="C16" s="19" t="s">
-        <v>110</v>
-      </c>
-      <c r="D16" s="19" t="s">
-        <v>111</v>
-      </c>
-      <c r="E16" s="19" t="s">
-        <v>103</v>
-      </c>
-      <c r="F16" s="19"/>
-      <c r="G16" s="19">
-        <v>2012</v>
-      </c>
-      <c r="H16" s="19" t="s">
-        <v>113</v>
-      </c>
-      <c r="I16" s="19">
-        <v>1</v>
-      </c>
-      <c r="J16" s="47"/>
-      <c r="K16" s="47"/>
-      <c r="L16" s="67">
-        <v>2.5599999999999998E-2</v>
-      </c>
-      <c r="M16" s="67">
-        <v>0.77777777777777779</v>
-      </c>
-      <c r="N16" s="47"/>
-      <c r="O16" s="47">
-        <v>25</v>
-      </c>
-      <c r="P16" s="65">
-        <v>3.1536000000000002E-2</v>
-      </c>
-      <c r="Q16" s="47"/>
-      <c r="R16" s="47"/>
-      <c r="S16" s="65">
-        <v>0.37</v>
-      </c>
-      <c r="T16" s="65">
-        <v>100</v>
-      </c>
-      <c r="U16" s="65">
-        <v>1</v>
-      </c>
-      <c r="V16" s="65"/>
-    </row>
-    <row r="17" spans="2:22" x14ac:dyDescent="0.2">
-      <c r="B17" s="19" t="s">
-        <v>143</v>
-      </c>
-      <c r="C17" s="19" t="s">
-        <v>144</v>
-      </c>
-      <c r="D17" s="19" t="s">
-        <v>145</v>
-      </c>
-      <c r="E17" s="19" t="s">
-        <v>108</v>
-      </c>
-      <c r="F17" s="19"/>
-      <c r="G17" s="19"/>
-      <c r="H17" s="19"/>
-      <c r="I17" s="19">
-        <v>1</v>
-      </c>
-      <c r="J17" s="19"/>
-      <c r="K17" s="19"/>
-      <c r="L17" s="65"/>
-      <c r="M17" s="19"/>
-      <c r="N17" s="19"/>
-      <c r="O17" s="65"/>
-      <c r="P17" s="19"/>
-      <c r="Q17" s="19"/>
-      <c r="R17" s="65"/>
-      <c r="S17" s="19"/>
-      <c r="T17" s="19"/>
-      <c r="U17" s="65"/>
-      <c r="V17" s="65"/>
-    </row>
-    <row r="18" spans="2:22" x14ac:dyDescent="0.2">
-      <c r="B18" s="19" t="s">
-        <v>146</v>
-      </c>
-      <c r="C18" s="19" t="s">
-        <v>147</v>
-      </c>
-      <c r="D18" s="19" t="s">
-        <v>148</v>
-      </c>
-      <c r="E18" s="19" t="s">
-        <v>111</v>
-      </c>
-      <c r="F18" s="19"/>
-      <c r="G18" s="19"/>
-      <c r="H18" s="19"/>
-      <c r="I18" s="19">
-        <v>1</v>
-      </c>
-      <c r="J18" s="19"/>
-      <c r="K18" s="19"/>
-      <c r="L18" s="65"/>
-      <c r="M18" s="19"/>
-      <c r="N18" s="19"/>
-      <c r="O18" s="65"/>
-      <c r="P18" s="19"/>
-      <c r="Q18" s="19"/>
-      <c r="R18" s="65"/>
-      <c r="S18" s="19"/>
-      <c r="T18" s="19"/>
-      <c r="U18" s="65"/>
-      <c r="V18" s="65"/>
-    </row>
-    <row r="19" spans="2:22" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="B19" s="45" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="22" spans="2:22" x14ac:dyDescent="0.2">
-      <c r="B22" s="23" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="23" spans="2:22" x14ac:dyDescent="0.2">
-      <c r="B23" s="22" t="s">
-        <v>0</v>
-      </c>
-      <c r="C23" s="22" t="s">
-        <v>84</v>
-      </c>
-      <c r="D23" s="22" t="s">
-        <v>82</v>
-      </c>
-      <c r="E23" s="22" t="s">
-        <v>80</v>
-      </c>
-      <c r="F23" s="1"/>
-    </row>
-    <row r="24" spans="2:22" ht="39" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="20" t="s">
+      <c r="C24" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="D24" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="E24" s="20" t="s">
         <v>48</v>
       </c>
-      <c r="C24" s="20" t="s">
-        <v>29</v>
-      </c>
-      <c r="D24" s="20" t="s">
-        <v>4</v>
-      </c>
-      <c r="E24" s="21" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="25" spans="2:22" x14ac:dyDescent="0.2">
-      <c r="B25" s="24"/>
-      <c r="C25" s="24"/>
-      <c r="D25" s="24"/>
-      <c r="E25" s="24"/>
-    </row>
-    <row r="26" spans="2:22" x14ac:dyDescent="0.2">
-      <c r="B26" s="19"/>
-      <c r="C26" s="19"/>
-      <c r="D26" s="19"/>
-      <c r="E26" s="19"/>
-    </row>
-    <row r="27" spans="2:22" x14ac:dyDescent="0.2">
-      <c r="B27" s="19"/>
-      <c r="C27" s="19"/>
-      <c r="D27" s="19"/>
-      <c r="E27" s="19"/>
-    </row>
-    <row r="28" spans="2:22" x14ac:dyDescent="0.2">
-      <c r="B28" s="19"/>
-      <c r="C28" s="19"/>
-      <c r="D28" s="19"/>
-      <c r="E28" s="19"/>
-    </row>
-    <row r="29" spans="2:22" x14ac:dyDescent="0.2">
-      <c r="B29" s="19"/>
-      <c r="C29" s="19"/>
-      <c r="D29" s="19"/>
-      <c r="E29" s="19"/>
-    </row>
-    <row r="30" spans="2:22" x14ac:dyDescent="0.2">
-      <c r="B30" s="19"/>
-      <c r="C30" s="19"/>
-      <c r="D30" s="19"/>
-      <c r="E30" s="19"/>
+    </row>
+    <row r="25" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B25" s="23"/>
+      <c r="C25" s="23"/>
+      <c r="D25" s="23"/>
+      <c r="E25" s="23"/>
+    </row>
+    <row r="26" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B26" s="18"/>
+      <c r="C26" s="18"/>
+      <c r="D26" s="18"/>
+      <c r="E26" s="18"/>
+    </row>
+    <row r="27" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B27" s="18"/>
+      <c r="C27" s="18"/>
+      <c r="D27" s="18"/>
+      <c r="E27" s="18"/>
+    </row>
+    <row r="28" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B28" s="18"/>
+      <c r="C28" s="18"/>
+      <c r="D28" s="18"/>
+      <c r="E28" s="18"/>
+    </row>
+    <row r="29" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B29" s="18"/>
+      <c r="C29" s="18"/>
+      <c r="D29" s="18"/>
+      <c r="E29" s="18"/>
+    </row>
+    <row r="30" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B30" s="18"/>
+      <c r="C30" s="18"/>
+      <c r="D30" s="18"/>
+      <c r="E30" s="18"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -3472,265 +3308,75 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K12"/>
+  <dimension ref="A4:F12"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7" style="33" customWidth="1"/>
-    <col min="2" max="2" width="15.5703125" style="33" customWidth="1"/>
-    <col min="3" max="3" width="11.7109375" style="33" customWidth="1"/>
-    <col min="4" max="4" width="12.140625" style="33" customWidth="1"/>
-    <col min="5" max="5" width="11.85546875" style="33" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="11.85546875" style="33" customWidth="1"/>
-    <col min="8" max="8" width="10.140625" style="33" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.5703125" style="33" customWidth="1"/>
-    <col min="10" max="10" width="11.28515625" style="33" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17.140625" style="33" bestFit="1" customWidth="1"/>
-    <col min="12" max="16384" width="9.140625" style="33"/>
+    <col min="2" max="2" width="33.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="28.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="33.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="B1" s="45" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B2"/>
-      <c r="H2"/>
-      <c r="I2"/>
-      <c r="J2"/>
-    </row>
-    <row r="3" spans="1:11" ht="18" x14ac:dyDescent="0.25">
-      <c r="B3" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="H3"/>
-      <c r="I3"/>
-      <c r="J3"/>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="H4"/>
-      <c r="I4"/>
-      <c r="J4"/>
-    </row>
-    <row r="5" spans="1:11" ht="15" x14ac:dyDescent="0.2">
-      <c r="B5" s="25" t="s">
-        <v>62</v>
-      </c>
-      <c r="C5"/>
-      <c r="D5"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="34"/>
-      <c r="G5" s="34"/>
-      <c r="K5" s="35"/>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B6" s="9"/>
-      <c r="C6" s="2"/>
-      <c r="D6"/>
-      <c r="E6" s="12"/>
-      <c r="F6" s="36"/>
-      <c r="G6" s="36"/>
-      <c r="K6" s="35"/>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B7"/>
-      <c r="C7"/>
-      <c r="D7"/>
-      <c r="E7"/>
-      <c r="I7" s="37"/>
-    </row>
-    <row r="8" spans="1:11" s="38" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="39" t="s">
-        <v>1</v>
-      </c>
-      <c r="C8" s="39" t="s">
-        <v>50</v>
-      </c>
-      <c r="D8" s="39" t="s">
-        <v>5</v>
-      </c>
-      <c r="E8" s="40" t="s">
-        <v>6</v>
-      </c>
-      <c r="F8" s="40" t="s">
-        <v>54</v>
-      </c>
-      <c r="G8" s="40" t="s">
-        <v>8</v>
-      </c>
-      <c r="H8" s="40" t="s">
-        <v>68</v>
-      </c>
-      <c r="I8" s="40" t="s">
-        <v>51</v>
-      </c>
-      <c r="J8" s="39" t="s">
-        <v>94</v>
-      </c>
-      <c r="K8" s="39" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" ht="38.85" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="41"/>
-      <c r="B9" s="59" t="s">
-        <v>59</v>
-      </c>
-      <c r="C9" s="59" t="s">
-        <v>24</v>
-      </c>
-      <c r="D9" s="59" t="s">
-        <v>37</v>
-      </c>
-      <c r="E9" s="59" t="s">
-        <v>38</v>
-      </c>
-      <c r="F9" s="59" t="s">
-        <v>55</v>
-      </c>
-      <c r="G9" s="59" t="s">
-        <v>56</v>
-      </c>
-      <c r="H9" s="59"/>
-      <c r="I9" s="59" t="s">
-        <v>52</v>
-      </c>
-      <c r="J9" s="59" t="s">
-        <v>53</v>
-      </c>
-      <c r="K9" s="59" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" ht="15.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="41"/>
-      <c r="B10" s="63" t="s">
-        <v>82</v>
-      </c>
-      <c r="C10" s="64"/>
-      <c r="D10" s="64"/>
-      <c r="E10" s="64"/>
-      <c r="F10" s="64"/>
-      <c r="G10" s="63"/>
-      <c r="H10" s="63"/>
-      <c r="I10" s="63"/>
-      <c r="J10" s="63"/>
-      <c r="K10" s="63"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B11" s="42"/>
-      <c r="C11" s="42"/>
-      <c r="D11" s="43"/>
-      <c r="E11" s="43"/>
-      <c r="F11" s="43"/>
-      <c r="G11" s="43"/>
-      <c r="H11" s="43"/>
-      <c r="I11" s="44" t="s">
-        <v>81</v>
-      </c>
-      <c r="J11" s="46"/>
-      <c r="K11" s="46"/>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B12" s="42"/>
-      <c r="C12" s="42"/>
-      <c r="D12" s="43"/>
-      <c r="E12" s="43"/>
-      <c r="F12" s="43"/>
-      <c r="G12" s="43"/>
-      <c r="H12" s="43"/>
-      <c r="I12" s="44" t="s">
-        <v>73</v>
-      </c>
-      <c r="J12" s="46"/>
-      <c r="K12" s="46"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292"/>
-  <headerFooter alignWithMargins="0"/>
-  <legacyDrawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A4:F12"/>
-  <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="2" max="2" width="33.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="5" width="28.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="33.85546875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="4" spans="1:6" ht="15" x14ac:dyDescent="0.2">
-      <c r="A4" s="13" t="s">
+    <row r="4" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A4" s="12" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="16"/>
+      <c r="C6" s="15"/>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
     </row>
-    <row r="7" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="17" t="s">
+    <row r="7" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="C7" s="18" t="s">
-        <v>100</v>
-      </c>
-      <c r="D7" s="18" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="15" t="s">
-        <v>43</v>
-      </c>
-      <c r="C8" s="73" t="s">
-        <v>141</v>
-      </c>
-      <c r="D8" s="73" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B9" s="19" t="s">
-        <v>133</v>
-      </c>
-      <c r="C9" s="65">
+      <c r="C7" s="17" t="s">
+        <v>88</v>
+      </c>
+      <c r="D7" s="17" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="C8" s="59" t="s">
+        <v>129</v>
+      </c>
+      <c r="D8" s="59" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B9" s="18" t="s">
+        <v>121</v>
+      </c>
+      <c r="C9" s="51">
         <v>94.6</v>
       </c>
-      <c r="D9" s="65">
+      <c r="D9" s="51">
         <v>57</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B10" s="1" t="s">
-        <v>42</v>
-      </c>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B10" s="1"/>
       <c r="C10" s="1"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
     </row>

</xml_diff>

<commit_message>
Units added in the "ProcessCharac" sheet
Attributes not used and not shown in the tutorials removed from the "ProcessCharac"
</commit_message>
<xml_diff>
--- a/VT_SHR_ELC_V01.xlsx
+++ b/VT_SHR_ELC_V01.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="9552" yWindow="-12" windowWidth="4128" windowHeight="9408" tabRatio="901"/>
+    <workbookView xWindow="9552" yWindow="-12" windowWidth="4128" windowHeight="9408" tabRatio="901" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="SEC_Comm" sheetId="112" r:id="rId1"/>
@@ -23,7 +23,7 @@
   <definedNames>
     <definedName name="FID_1">[1]AGR_Fuels!$A$2</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -793,53 +793,6 @@
         </r>
       </text>
     </comment>
-    <comment ref="Q8" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">This attribute is used to assign a production limit.
-By defautt is defined like fixed share
-</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>UP</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-If you want fix or lower add
-</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>~FX
-~LO</t>
-        </r>
-      </text>
-    </comment>
   </commentList>
 </comments>
 </file>
@@ -868,7 +821,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="128">
   <si>
     <t>CommName</t>
   </si>
@@ -1053,48 +1006,27 @@
     <t>CURR</t>
   </si>
   <si>
-    <t>Comm-IN-A</t>
-  </si>
-  <si>
-    <t>FLO_COST</t>
-  </si>
-  <si>
     <t>~FI_T:</t>
   </si>
   <si>
     <t>Typical structure used to specify base-year demand levels</t>
   </si>
   <si>
-    <t>ACT_BND</t>
-  </si>
-  <si>
     <t>ACT_COST</t>
   </si>
   <si>
-    <t>NCAP_COST</t>
-  </si>
-  <si>
     <t>PRC_CAPACT</t>
   </si>
   <si>
-    <t>FLO_SHAR~UP</t>
-  </si>
-  <si>
     <t>NCAP_FOM</t>
   </si>
   <si>
-    <t>VDA_FLOP</t>
-  </si>
-  <si>
     <t>COM_PROJ</t>
   </si>
   <si>
     <t>*Unit</t>
   </si>
   <si>
-    <t>Process Activiity Bound</t>
-  </si>
-  <si>
     <t>*CommDesc</t>
   </si>
   <si>
@@ -1104,21 +1036,6 @@
     <t>Currency</t>
   </si>
   <si>
-    <t>Auxiliary Input Commodity</t>
-  </si>
-  <si>
-    <t>Process Input Tied to Activity</t>
-  </si>
-  <si>
-    <t>Share of a Ccommodity in a Group</t>
-  </si>
-  <si>
-    <t>Annual Delivery Cost</t>
-  </si>
-  <si>
-    <t>Capacity Investment Cost</t>
-  </si>
-  <si>
     <t>NCAP_TLIFE</t>
   </si>
   <si>
@@ -1279,6 +1196,15 @@
   </si>
   <si>
     <t>WIN</t>
+  </si>
+  <si>
+    <t>Meuro/MW</t>
+  </si>
+  <si>
+    <t>Meuro/PJ</t>
+  </si>
+  <si>
+    <t>Years</t>
   </si>
 </sst>
 </file>
@@ -1522,7 +1448,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1620,9 +1546,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2158,8 +2081,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="B1:J13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -2275,84 +2198,84 @@
       </c>
     </row>
     <row r="10" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B10" s="51" t="s">
-        <v>120</v>
-      </c>
-      <c r="C10" s="58"/>
-      <c r="D10" s="51" t="s">
-        <v>121</v>
-      </c>
-      <c r="E10" s="51" t="s">
-        <v>122</v>
-      </c>
-      <c r="F10" s="51" t="s">
-        <v>123</v>
-      </c>
-      <c r="G10" s="51"/>
-      <c r="H10" s="51" t="s">
-        <v>124</v>
-      </c>
-      <c r="I10" s="51"/>
-      <c r="J10" s="51"/>
+      <c r="B10" s="50" t="s">
+        <v>108</v>
+      </c>
+      <c r="C10" s="57"/>
+      <c r="D10" s="50" t="s">
+        <v>109</v>
+      </c>
+      <c r="E10" s="50" t="s">
+        <v>110</v>
+      </c>
+      <c r="F10" s="50" t="s">
+        <v>111</v>
+      </c>
+      <c r="G10" s="50"/>
+      <c r="H10" s="50" t="s">
+        <v>112</v>
+      </c>
+      <c r="I10" s="50"/>
+      <c r="J10" s="50"/>
     </row>
     <row r="11" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B11" s="51" t="s">
-        <v>125</v>
-      </c>
-      <c r="C11" s="58"/>
-      <c r="D11" s="51" t="s">
-        <v>88</v>
-      </c>
-      <c r="E11" s="51" t="s">
-        <v>126</v>
-      </c>
-      <c r="F11" s="51" t="s">
+      <c r="B11" s="50" t="s">
+        <v>113</v>
+      </c>
+      <c r="C11" s="57"/>
+      <c r="D11" s="50" t="s">
+        <v>76</v>
+      </c>
+      <c r="E11" s="50" t="s">
         <v>114</v>
       </c>
-      <c r="G11" s="51" t="s">
-        <v>117</v>
-      </c>
-      <c r="H11" s="51"/>
-      <c r="I11" s="51"/>
-      <c r="J11" s="51"/>
+      <c r="F11" s="50" t="s">
+        <v>102</v>
+      </c>
+      <c r="G11" s="50" t="s">
+        <v>105</v>
+      </c>
+      <c r="H11" s="50"/>
+      <c r="I11" s="50"/>
+      <c r="J11" s="50"/>
     </row>
     <row r="12" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B12" s="51" t="s">
-        <v>125</v>
-      </c>
-      <c r="C12" s="58"/>
-      <c r="D12" s="51" t="s">
-        <v>96</v>
-      </c>
-      <c r="E12" s="51" t="s">
-        <v>127</v>
-      </c>
-      <c r="F12" s="51" t="s">
-        <v>114</v>
-      </c>
-      <c r="G12" s="51"/>
-      <c r="H12" s="51"/>
-      <c r="I12" s="51"/>
-      <c r="J12" s="51"/>
+      <c r="B12" s="50" t="s">
+        <v>113</v>
+      </c>
+      <c r="C12" s="57"/>
+      <c r="D12" s="50" t="s">
+        <v>84</v>
+      </c>
+      <c r="E12" s="50" t="s">
+        <v>115</v>
+      </c>
+      <c r="F12" s="50" t="s">
+        <v>102</v>
+      </c>
+      <c r="G12" s="50"/>
+      <c r="H12" s="50"/>
+      <c r="I12" s="50"/>
+      <c r="J12" s="50"/>
     </row>
     <row r="13" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B13" s="51" t="s">
-        <v>125</v>
-      </c>
-      <c r="C13" s="58"/>
-      <c r="D13" s="51" t="s">
-        <v>99</v>
-      </c>
-      <c r="E13" s="51" t="s">
-        <v>128</v>
-      </c>
-      <c r="F13" s="51" t="s">
-        <v>114</v>
-      </c>
-      <c r="G13" s="51"/>
-      <c r="H13" s="51"/>
-      <c r="I13" s="51"/>
-      <c r="J13" s="51"/>
+      <c r="B13" s="50" t="s">
+        <v>113</v>
+      </c>
+      <c r="C13" s="57"/>
+      <c r="D13" s="50" t="s">
+        <v>87</v>
+      </c>
+      <c r="E13" s="50" t="s">
+        <v>116</v>
+      </c>
+      <c r="F13" s="50" t="s">
+        <v>102</v>
+      </c>
+      <c r="G13" s="50"/>
+      <c r="H13" s="50"/>
+      <c r="I13" s="50"/>
+      <c r="J13" s="50"/>
     </row>
   </sheetData>
   <phoneticPr fontId="0" type="noConversion"/>
@@ -2482,161 +2405,161 @@
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B9" s="58" t="s">
-        <v>112</v>
-      </c>
-      <c r="C9" s="58"/>
-      <c r="D9" s="58" t="s">
-        <v>89</v>
-      </c>
-      <c r="E9" s="58" t="s">
-        <v>113</v>
-      </c>
-      <c r="F9" s="58" t="s">
-        <v>114</v>
-      </c>
-      <c r="G9" s="58" t="s">
-        <v>111</v>
-      </c>
-      <c r="H9" s="58"/>
-      <c r="I9" s="58"/>
-      <c r="J9" s="58"/>
+      <c r="B9" s="57" t="s">
+        <v>100</v>
+      </c>
+      <c r="C9" s="57"/>
+      <c r="D9" s="57" t="s">
+        <v>77</v>
+      </c>
+      <c r="E9" s="57" t="s">
+        <v>101</v>
+      </c>
+      <c r="F9" s="57" t="s">
+        <v>102</v>
+      </c>
+      <c r="G9" s="57" t="s">
+        <v>99</v>
+      </c>
+      <c r="H9" s="57"/>
+      <c r="I9" s="57"/>
+      <c r="J9" s="57"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B10" s="58" t="s">
-        <v>115</v>
-      </c>
-      <c r="C10" s="58"/>
-      <c r="D10" s="58" t="s">
+      <c r="B10" s="57" t="s">
+        <v>103</v>
+      </c>
+      <c r="C10" s="57"/>
+      <c r="D10" s="57" t="s">
+        <v>73</v>
+      </c>
+      <c r="E10" s="57" t="s">
+        <v>74</v>
+      </c>
+      <c r="F10" s="57" t="s">
+        <v>102</v>
+      </c>
+      <c r="G10" s="57" t="s">
+        <v>104</v>
+      </c>
+      <c r="H10" s="57" t="s">
+        <v>105</v>
+      </c>
+      <c r="I10" s="57"/>
+      <c r="J10" s="57"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B11" s="57" t="s">
+        <v>106</v>
+      </c>
+      <c r="C11" s="57"/>
+      <c r="D11" s="57" t="s">
+        <v>118</v>
+      </c>
+      <c r="E11" s="57" t="s">
+        <v>80</v>
+      </c>
+      <c r="F11" s="57" t="s">
+        <v>102</v>
+      </c>
+      <c r="G11" s="57" t="s">
+        <v>99</v>
+      </c>
+      <c r="H11" s="57"/>
+      <c r="I11" s="57"/>
+      <c r="J11" s="57"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B12" s="57" t="s">
+        <v>107</v>
+      </c>
+      <c r="C12" s="57"/>
+      <c r="D12" s="57" t="s">
+        <v>82</v>
+      </c>
+      <c r="E12" s="57" t="s">
+        <v>83</v>
+      </c>
+      <c r="F12" s="57" t="s">
+        <v>102</v>
+      </c>
+      <c r="G12" s="57" t="s">
+        <v>99</v>
+      </c>
+      <c r="H12" s="57"/>
+      <c r="I12" s="57"/>
+      <c r="J12" s="57"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B13" s="57" t="s">
+        <v>107</v>
+      </c>
+      <c r="C13" s="57"/>
+      <c r="D13" s="57" t="s">
         <v>85</v>
       </c>
-      <c r="E10" s="58" t="s">
+      <c r="E13" s="57" t="s">
         <v>86</v>
       </c>
-      <c r="F10" s="58" t="s">
-        <v>114</v>
-      </c>
-      <c r="G10" s="58" t="s">
-        <v>116</v>
-      </c>
-      <c r="H10" s="58" t="s">
-        <v>117</v>
-      </c>
-      <c r="I10" s="58"/>
-      <c r="J10" s="58"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B11" s="58" t="s">
-        <v>118</v>
-      </c>
-      <c r="C11" s="58"/>
-      <c r="D11" s="58" t="s">
-        <v>130</v>
-      </c>
-      <c r="E11" s="58" t="s">
-        <v>92</v>
-      </c>
-      <c r="F11" s="58" t="s">
-        <v>114</v>
-      </c>
-      <c r="G11" s="58" t="s">
-        <v>111</v>
-      </c>
-      <c r="H11" s="58"/>
-      <c r="I11" s="58"/>
-      <c r="J11" s="58"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B12" s="58" t="s">
-        <v>119</v>
-      </c>
-      <c r="C12" s="58"/>
-      <c r="D12" s="58" t="s">
-        <v>94</v>
-      </c>
-      <c r="E12" s="58" t="s">
-        <v>95</v>
-      </c>
-      <c r="F12" s="58" t="s">
-        <v>114</v>
-      </c>
-      <c r="G12" s="58" t="s">
-        <v>111</v>
-      </c>
-      <c r="H12" s="58"/>
-      <c r="I12" s="58"/>
-      <c r="J12" s="58"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B13" s="58" t="s">
-        <v>119</v>
-      </c>
-      <c r="C13" s="58"/>
-      <c r="D13" s="58" t="s">
-        <v>97</v>
-      </c>
-      <c r="E13" s="58" t="s">
-        <v>98</v>
-      </c>
-      <c r="F13" s="58" t="s">
-        <v>114</v>
-      </c>
-      <c r="G13" s="58" t="s">
-        <v>111</v>
-      </c>
-      <c r="H13" s="58"/>
-      <c r="I13" s="58"/>
-      <c r="J13" s="58"/>
+      <c r="F13" s="57" t="s">
+        <v>102</v>
+      </c>
+      <c r="G13" s="57" t="s">
+        <v>99</v>
+      </c>
+      <c r="H13" s="57"/>
+      <c r="I13" s="57"/>
+      <c r="J13" s="57"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B14" s="58" t="s">
-        <v>115</v>
-      </c>
-      <c r="C14" s="58"/>
-      <c r="D14" s="58" t="str">
+      <c r="B14" s="57" t="s">
+        <v>103</v>
+      </c>
+      <c r="C14" s="57"/>
+      <c r="D14" s="57" t="str">
         <f>ProcessCharac!B17</f>
         <v>FT-ELCNGA</v>
       </c>
-      <c r="E14" s="58" t="str">
+      <c r="E14" s="57" t="str">
         <f>ProcessCharac!C17</f>
         <v>Fuel Technology Natural Gas ELC</v>
       </c>
-      <c r="F14" s="58" t="s">
-        <v>114</v>
-      </c>
-      <c r="G14" s="58" t="s">
-        <v>116</v>
-      </c>
-      <c r="H14" s="58" t="s">
-        <v>117</v>
-      </c>
-      <c r="I14" s="58"/>
-      <c r="J14" s="58"/>
+      <c r="F14" s="57" t="s">
+        <v>102</v>
+      </c>
+      <c r="G14" s="57" t="s">
+        <v>104</v>
+      </c>
+      <c r="H14" s="57" t="s">
+        <v>105</v>
+      </c>
+      <c r="I14" s="57"/>
+      <c r="J14" s="57"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B15" s="58" t="s">
-        <v>115</v>
-      </c>
-      <c r="C15" s="58"/>
-      <c r="D15" s="58" t="str">
+      <c r="B15" s="57" t="s">
+        <v>103</v>
+      </c>
+      <c r="C15" s="57"/>
+      <c r="D15" s="57" t="str">
         <f>ProcessCharac!B18</f>
         <v>FT-ELCWIN</v>
       </c>
-      <c r="E15" s="58" t="str">
+      <c r="E15" s="57" t="str">
         <f>ProcessCharac!C18</f>
         <v>Fuel Technology Wind ELC</v>
       </c>
-      <c r="F15" s="58" t="s">
-        <v>114</v>
-      </c>
-      <c r="G15" s="58" t="s">
-        <v>116</v>
-      </c>
-      <c r="H15" s="58" t="s">
-        <v>117</v>
-      </c>
-      <c r="I15" s="58"/>
-      <c r="J15" s="58"/>
+      <c r="F15" s="57" t="s">
+        <v>102</v>
+      </c>
+      <c r="G15" s="57" t="s">
+        <v>104</v>
+      </c>
+      <c r="H15" s="57" t="s">
+        <v>105</v>
+      </c>
+      <c r="I15" s="57"/>
+      <c r="J15" s="57"/>
     </row>
   </sheetData>
   <phoneticPr fontId="0" type="noConversion"/>
@@ -2649,10 +2572,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:V30"/>
+  <dimension ref="B1:S30"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F37" sqref="F37"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="Q12" sqref="Q12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -2660,13 +2583,19 @@
     <col min="1" max="1" width="5.88671875" customWidth="1"/>
     <col min="2" max="2" width="15.5546875" customWidth="1"/>
     <col min="3" max="3" width="43.44140625" customWidth="1"/>
-    <col min="4" max="9" width="11.6640625" customWidth="1"/>
-    <col min="10" max="10" width="11.109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.109375" customWidth="1"/>
-    <col min="12" max="12" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.6640625" customWidth="1"/>
+    <col min="5" max="5" width="12.44140625" customWidth="1"/>
+    <col min="6" max="6" width="5.44140625" customWidth="1"/>
+    <col min="7" max="7" width="10.44140625" customWidth="1"/>
+    <col min="8" max="8" width="11.6640625" customWidth="1"/>
+    <col min="9" max="9" width="12.88671875" customWidth="1"/>
+    <col min="10" max="10" width="12.6640625" customWidth="1"/>
+    <col min="11" max="11" width="14.44140625" customWidth="1"/>
+    <col min="12" max="12" width="15.5546875" customWidth="1"/>
     <col min="13" max="13" width="12.109375" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="13.44140625" bestFit="1" customWidth="1"/>
-    <col min="15" max="17" width="13.5546875" customWidth="1"/>
+    <col min="15" max="15" width="15.5546875" customWidth="1"/>
+    <col min="16" max="17" width="13.5546875" customWidth="1"/>
     <col min="18" max="18" width="18.6640625" customWidth="1"/>
     <col min="19" max="19" width="14.109375" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="13.44140625" customWidth="1"/>
@@ -2675,17 +2604,17 @@
     <col min="23" max="24" width="10.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:22" ht="24.6" x14ac:dyDescent="0.4">
+    <row r="1" spans="2:19" ht="24.6" x14ac:dyDescent="0.4">
       <c r="B1" s="32" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="3" spans="2:22" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:19" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="B3" s="13" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="5" spans="2:22" ht="15" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:19" ht="15" x14ac:dyDescent="0.25">
       <c r="B5" s="24" t="s">
         <v>55</v>
       </c>
@@ -2701,7 +2630,7 @@
       <c r="Q5" s="6"/>
       <c r="R5" s="6"/>
     </row>
-    <row r="6" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B6" s="9"/>
       <c r="C6" s="2"/>
       <c r="E6" s="4"/>
@@ -2717,24 +2646,23 @@
       <c r="R6" s="6"/>
       <c r="S6" s="6"/>
     </row>
-    <row r="7" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="F7" s="29"/>
-      <c r="H7" s="29" t="s">
+    <row r="7" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="G7" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="I7" s="29"/>
-      <c r="J7" s="30"/>
+      <c r="H7" s="29"/>
+      <c r="I7" s="30"/>
+      <c r="J7" s="26"/>
       <c r="K7" s="26"/>
-      <c r="L7" s="26"/>
-      <c r="M7" s="31"/>
-      <c r="N7" s="25"/>
-      <c r="O7" s="27"/>
-      <c r="P7" s="28"/>
+      <c r="L7" s="31"/>
+      <c r="M7" s="25"/>
+      <c r="N7" s="27"/>
+      <c r="O7" s="28"/>
+      <c r="P7" s="25"/>
       <c r="Q7" s="25"/>
-      <c r="R7" s="25"/>
-      <c r="S7" s="27"/>
-    </row>
-    <row r="8" spans="2:22" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="R7" s="27"/>
+    </row>
+    <row r="8" spans="2:19" s="1" customFormat="1" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="46" t="s">
         <v>1</v>
       </c>
@@ -2748,58 +2676,40 @@
         <v>6</v>
       </c>
       <c r="F8" s="46" t="s">
-        <v>61</v>
+        <v>69</v>
       </c>
       <c r="G8" s="46" t="s">
-        <v>76</v>
-      </c>
-      <c r="H8" s="46" t="s">
         <v>60</v>
       </c>
+      <c r="H8" s="34" t="s">
+        <v>15</v>
+      </c>
       <c r="I8" s="34" t="s">
-        <v>15</v>
+        <v>65</v>
       </c>
       <c r="J8" s="34" t="s">
+        <v>63</v>
+      </c>
+      <c r="K8" s="34" t="s">
         <v>71</v>
       </c>
-      <c r="K8" s="34" t="s">
-        <v>62</v>
-      </c>
       <c r="L8" s="34" t="s">
-        <v>70</v>
-      </c>
-      <c r="M8" s="34" t="s">
-        <v>66</v>
-      </c>
-      <c r="N8" s="34" t="s">
-        <v>67</v>
-      </c>
-      <c r="O8" s="34" t="s">
-        <v>83</v>
-      </c>
-      <c r="P8" s="34" t="s">
-        <v>68</v>
-      </c>
-      <c r="Q8" s="48" t="s">
-        <v>65</v>
-      </c>
-      <c r="R8" s="34" t="s">
-        <v>69</v>
-      </c>
-      <c r="S8" s="54" t="s">
-        <v>102</v>
-      </c>
-      <c r="T8" s="54" t="s">
-        <v>103</v>
-      </c>
-      <c r="U8" s="54" t="s">
-        <v>104</v>
-      </c>
-      <c r="V8" s="54" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="9" spans="2:22" ht="42.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>64</v>
+      </c>
+      <c r="M8" s="53" t="s">
+        <v>90</v>
+      </c>
+      <c r="N8" s="53" t="s">
+        <v>91</v>
+      </c>
+      <c r="O8" s="53" t="s">
+        <v>92</v>
+      </c>
+      <c r="P8" s="53" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="9" spans="2:19" ht="54.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B9" s="45" t="s">
         <v>52</v>
       </c>
@@ -2813,442 +2723,382 @@
         <v>38</v>
       </c>
       <c r="F9" s="45" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="G9" s="45" t="s">
+        <v>70</v>
+      </c>
+      <c r="H9" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="I9" s="45" t="s">
+        <v>46</v>
+      </c>
+      <c r="J9" s="45" t="s">
+        <v>45</v>
+      </c>
+      <c r="K9" s="45" t="s">
+        <v>72</v>
+      </c>
+      <c r="L9" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="M9" s="54" t="s">
+        <v>94</v>
+      </c>
+      <c r="N9" s="54" t="s">
+        <v>95</v>
+      </c>
+      <c r="O9" s="54" t="s">
+        <v>96</v>
+      </c>
+      <c r="P9" s="54" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="10" spans="2:19" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B10" s="48" t="s">
+        <v>67</v>
+      </c>
+      <c r="C10" s="49"/>
+      <c r="D10" s="49"/>
+      <c r="E10" s="49"/>
+      <c r="F10" s="48"/>
+      <c r="G10" s="48" t="s">
+        <v>70</v>
+      </c>
+      <c r="H10" s="48" t="s">
+        <v>98</v>
+      </c>
+      <c r="I10" s="48" t="s">
+        <v>125</v>
+      </c>
+      <c r="J10" s="48" t="s">
+        <v>126</v>
+      </c>
+      <c r="K10" s="49" t="s">
+        <v>127</v>
+      </c>
+      <c r="L10" s="48" t="s">
+        <v>98</v>
+      </c>
+      <c r="M10" s="55" t="s">
+        <v>98</v>
+      </c>
+      <c r="N10" s="55" t="s">
+        <v>99</v>
+      </c>
+      <c r="O10" s="56"/>
+      <c r="P10" s="56"/>
+    </row>
+    <row r="11" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B11" s="18" t="s">
+        <v>73</v>
+      </c>
+      <c r="C11" s="18" t="s">
+        <v>74</v>
+      </c>
+      <c r="D11" s="18" t="s">
+        <v>75</v>
+      </c>
+      <c r="E11" s="18" t="s">
         <v>76</v>
-      </c>
-      <c r="H9" s="45" t="s">
-        <v>77</v>
-      </c>
-      <c r="I9" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="J9" s="45" t="s">
-        <v>79</v>
-      </c>
-      <c r="K9" s="45" t="s">
-        <v>81</v>
-      </c>
-      <c r="L9" s="45" t="s">
-        <v>46</v>
-      </c>
-      <c r="M9" s="45" t="s">
-        <v>45</v>
-      </c>
-      <c r="N9" s="45" t="s">
-        <v>82</v>
-      </c>
-      <c r="O9" s="45" t="s">
-        <v>84</v>
-      </c>
-      <c r="P9" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="Q9" s="45" t="s">
-        <v>74</v>
-      </c>
-      <c r="R9" s="45" t="s">
-        <v>80</v>
-      </c>
-      <c r="S9" s="55" t="s">
-        <v>106</v>
-      </c>
-      <c r="T9" s="55" t="s">
-        <v>107</v>
-      </c>
-      <c r="U9" s="55" t="s">
-        <v>108</v>
-      </c>
-      <c r="V9" s="55" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="10" spans="2:22" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B10" s="49" t="s">
-        <v>73</v>
-      </c>
-      <c r="C10" s="50"/>
-      <c r="D10" s="50"/>
-      <c r="E10" s="50"/>
-      <c r="F10" s="50"/>
-      <c r="G10" s="49"/>
-      <c r="H10" s="49"/>
-      <c r="I10" s="49"/>
-      <c r="J10" s="49"/>
-      <c r="K10" s="49"/>
-      <c r="L10" s="49"/>
-      <c r="M10" s="49"/>
-      <c r="N10" s="49"/>
-      <c r="O10" s="50"/>
-      <c r="P10" s="49"/>
-      <c r="Q10" s="50"/>
-      <c r="R10" s="50"/>
-      <c r="S10" s="56" t="s">
-        <v>110</v>
-      </c>
-      <c r="T10" s="56" t="s">
-        <v>111</v>
-      </c>
-      <c r="U10" s="57"/>
-      <c r="V10" s="57"/>
-    </row>
-    <row r="11" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B11" s="18" t="s">
-        <v>85</v>
-      </c>
-      <c r="C11" s="18" t="s">
-        <v>86</v>
-      </c>
-      <c r="D11" s="18" t="s">
-        <v>87</v>
-      </c>
-      <c r="E11" s="18" t="s">
-        <v>88</v>
       </c>
       <c r="F11" s="18"/>
       <c r="G11" s="18"/>
-      <c r="H11" s="18"/>
-      <c r="I11" s="18">
+      <c r="H11" s="18">
         <v>1</v>
       </c>
-      <c r="J11" s="18"/>
+      <c r="I11" s="50"/>
+      <c r="J11" s="50"/>
       <c r="K11" s="18"/>
-      <c r="L11" s="51"/>
-      <c r="M11" s="51"/>
-      <c r="N11" s="18"/>
-      <c r="O11" s="18"/>
-      <c r="P11" s="51"/>
-      <c r="Q11" s="18"/>
-      <c r="R11" s="18"/>
-      <c r="S11" s="51"/>
-      <c r="T11" s="51"/>
-      <c r="U11" s="51"/>
-      <c r="V11" s="51"/>
-    </row>
-    <row r="12" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="L11" s="50"/>
+      <c r="M11" s="50"/>
+      <c r="N11" s="50"/>
+      <c r="O11" s="50"/>
+      <c r="P11" s="50"/>
+    </row>
+    <row r="12" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B12" s="18" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
       <c r="C12" s="18" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="D12" s="18" t="s">
+        <v>76</v>
+      </c>
+      <c r="E12" s="18" t="s">
+        <v>79</v>
+      </c>
+      <c r="F12" s="18">
+        <v>2012</v>
+      </c>
+      <c r="G12" s="18" t="s">
         <v>88</v>
       </c>
-      <c r="E12" s="18" t="s">
-        <v>91</v>
-      </c>
-      <c r="F12" s="18"/>
-      <c r="G12" s="18">
+      <c r="H12" s="18">
+        <v>0.437</v>
+      </c>
+      <c r="I12" s="50">
+        <v>2.145E-2</v>
+      </c>
+      <c r="J12" s="50">
+        <v>0.93089999999999995</v>
+      </c>
+      <c r="K12" s="18">
+        <v>40</v>
+      </c>
+      <c r="L12" s="50">
+        <v>3.1536000000000002E-2</v>
+      </c>
+      <c r="M12" s="50">
+        <v>0.85099999999999998</v>
+      </c>
+      <c r="N12" s="50">
+        <v>108.2</v>
+      </c>
+      <c r="O12" s="50">
+        <v>1</v>
+      </c>
+      <c r="P12" s="50"/>
+    </row>
+    <row r="13" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B13" s="18" t="s">
+        <v>118</v>
+      </c>
+      <c r="C13" s="18" t="s">
+        <v>80</v>
+      </c>
+      <c r="D13" s="18" t="s">
+        <v>76</v>
+      </c>
+      <c r="E13" s="18" t="s">
+        <v>79</v>
+      </c>
+      <c r="F13" s="18">
         <v>2012</v>
       </c>
-      <c r="H12" s="18" t="s">
-        <v>100</v>
-      </c>
-      <c r="I12" s="18">
-        <v>0.437</v>
-      </c>
-      <c r="J12" s="18"/>
-      <c r="K12" s="33"/>
-      <c r="L12" s="51">
-        <v>2.145E-2</v>
-      </c>
-      <c r="M12" s="51">
-        <v>0.93089999999999995</v>
-      </c>
-      <c r="N12" s="18"/>
-      <c r="O12" s="18">
-        <v>40</v>
-      </c>
-      <c r="P12" s="51">
+      <c r="G13" s="18" t="s">
+        <v>88</v>
+      </c>
+      <c r="H13" s="18">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="I13" s="51">
+        <v>0.1</v>
+      </c>
+      <c r="J13" s="51">
+        <v>0.6</v>
+      </c>
+      <c r="K13" s="18">
+        <v>35</v>
+      </c>
+      <c r="L13" s="50">
         <v>3.1536000000000002E-2</v>
       </c>
-      <c r="Q12" s="18"/>
-      <c r="R12" s="33"/>
-      <c r="S12" s="51">
-        <v>0.85099999999999998</v>
-      </c>
-      <c r="T12" s="51">
-        <v>108.2</v>
-      </c>
-      <c r="U12" s="51">
+      <c r="M13" s="50">
+        <v>0.86</v>
+      </c>
+      <c r="N13" s="50">
+        <v>90000</v>
+      </c>
+      <c r="O13" s="50">
         <v>1</v>
       </c>
-      <c r="V12" s="51"/>
-    </row>
-    <row r="13" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B13" s="18" t="s">
-        <v>130</v>
-      </c>
-      <c r="C13" s="18" t="s">
-        <v>92</v>
-      </c>
-      <c r="D13" s="18" t="s">
-        <v>88</v>
-      </c>
-      <c r="E13" s="18" t="s">
-        <v>91</v>
-      </c>
-      <c r="F13" s="18"/>
-      <c r="G13" s="18">
-        <v>2012</v>
-      </c>
-      <c r="H13" s="18" t="s">
-        <v>100</v>
-      </c>
-      <c r="I13" s="18">
-        <v>0.28000000000000003</v>
-      </c>
-      <c r="J13" s="18"/>
-      <c r="K13" s="33"/>
-      <c r="L13" s="52">
-        <v>0.1</v>
-      </c>
-      <c r="M13" s="52">
-        <v>0.6</v>
-      </c>
-      <c r="N13" s="18"/>
-      <c r="O13" s="18">
-        <v>35</v>
-      </c>
-      <c r="P13" s="51">
-        <v>3.1536000000000002E-2</v>
-      </c>
-      <c r="Q13" s="18"/>
-      <c r="R13" s="33"/>
-      <c r="S13" s="51">
-        <v>0.86</v>
-      </c>
-      <c r="T13" s="51">
-        <v>90000</v>
-      </c>
-      <c r="U13" s="51">
-        <v>1</v>
-      </c>
-      <c r="V13" s="51">
+      <c r="P13" s="50">
         <v>2.1</v>
       </c>
     </row>
-    <row r="14" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B14" s="18"/>
       <c r="C14" s="18"/>
       <c r="D14" s="18"/>
       <c r="E14" s="18" t="s">
-        <v>93</v>
+        <v>81</v>
       </c>
       <c r="F14" s="18"/>
       <c r="G14" s="18"/>
       <c r="H14" s="18"/>
-      <c r="I14" s="18"/>
-      <c r="J14" s="18"/>
-      <c r="K14" s="33"/>
-      <c r="L14" s="51"/>
-      <c r="M14" s="51"/>
-      <c r="N14" s="18"/>
-      <c r="O14" s="18"/>
-      <c r="P14" s="51"/>
-      <c r="Q14" s="18"/>
-      <c r="R14" s="33"/>
-      <c r="S14" s="51"/>
-      <c r="T14" s="51"/>
-      <c r="U14" s="51"/>
-      <c r="V14" s="51"/>
-    </row>
-    <row r="15" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="I14" s="50"/>
+      <c r="J14" s="50"/>
+      <c r="K14" s="18"/>
+      <c r="L14" s="50"/>
+      <c r="M14" s="50"/>
+      <c r="N14" s="50"/>
+      <c r="O14" s="50"/>
+      <c r="P14" s="50"/>
+    </row>
+    <row r="15" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B15" s="18" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="C15" s="18" t="s">
-        <v>95</v>
+        <v>83</v>
       </c>
       <c r="D15" s="18" t="s">
-        <v>96</v>
+        <v>84</v>
       </c>
       <c r="E15" s="18" t="s">
-        <v>91</v>
-      </c>
-      <c r="F15" s="18"/>
-      <c r="G15" s="18">
+        <v>79</v>
+      </c>
+      <c r="F15" s="18">
         <v>2012</v>
       </c>
-      <c r="H15" s="18" t="s">
-        <v>101</v>
-      </c>
-      <c r="I15" s="18">
+      <c r="G15" s="18" t="s">
+        <v>89</v>
+      </c>
+      <c r="H15" s="18">
         <v>0.39</v>
       </c>
-      <c r="J15" s="18"/>
-      <c r="K15" s="33"/>
-      <c r="L15" s="51">
+      <c r="I15" s="50">
         <v>0.02</v>
       </c>
+      <c r="J15" s="50">
+        <v>1.25</v>
+      </c>
+      <c r="K15" s="18">
+        <v>25</v>
+      </c>
+      <c r="L15" s="50">
+        <v>3.1536000000000002E-2</v>
+      </c>
       <c r="M15" s="51">
-        <v>1.25</v>
-      </c>
-      <c r="N15" s="18"/>
-      <c r="O15" s="18">
+        <v>0.92346153799999997</v>
+      </c>
+      <c r="N15" s="50">
+        <v>100</v>
+      </c>
+      <c r="O15" s="50">
+        <v>1</v>
+      </c>
+      <c r="P15" s="50"/>
+    </row>
+    <row r="16" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B16" s="18" t="s">
+        <v>85</v>
+      </c>
+      <c r="C16" s="18" t="s">
+        <v>86</v>
+      </c>
+      <c r="D16" s="18" t="s">
+        <v>87</v>
+      </c>
+      <c r="E16" s="18" t="s">
+        <v>79</v>
+      </c>
+      <c r="F16" s="18">
+        <v>2012</v>
+      </c>
+      <c r="G16" s="18" t="s">
+        <v>89</v>
+      </c>
+      <c r="H16" s="18">
+        <v>1</v>
+      </c>
+      <c r="I16" s="52">
+        <v>2.5599999999999998E-2</v>
+      </c>
+      <c r="J16" s="52">
+        <v>0.77777777777777779</v>
+      </c>
+      <c r="K16" s="33">
         <v>25</v>
       </c>
-      <c r="P15" s="51">
+      <c r="L16" s="50">
         <v>3.1536000000000002E-2</v>
       </c>
-      <c r="Q15" s="18"/>
-      <c r="R15" s="33"/>
-      <c r="S15" s="52">
-        <v>0.92346153799999997</v>
-      </c>
-      <c r="T15" s="51">
+      <c r="M16" s="50">
+        <v>0.37</v>
+      </c>
+      <c r="N16" s="50">
         <v>100</v>
       </c>
-      <c r="U15" s="51">
+      <c r="O16" s="50">
         <v>1</v>
       </c>
-      <c r="V15" s="51"/>
-    </row>
-    <row r="16" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B16" s="18" t="s">
-        <v>97</v>
-      </c>
-      <c r="C16" s="18" t="s">
-        <v>98</v>
-      </c>
-      <c r="D16" s="18" t="s">
-        <v>99</v>
-      </c>
-      <c r="E16" s="18" t="s">
-        <v>91</v>
-      </c>
-      <c r="F16" s="18"/>
-      <c r="G16" s="18">
-        <v>2012</v>
-      </c>
-      <c r="H16" s="18" t="s">
-        <v>101</v>
-      </c>
-      <c r="I16" s="18">
-        <v>1</v>
-      </c>
-      <c r="J16" s="33"/>
-      <c r="K16" s="33"/>
-      <c r="L16" s="53">
-        <v>2.5599999999999998E-2</v>
-      </c>
-      <c r="M16" s="53">
-        <v>0.77777777777777779</v>
-      </c>
-      <c r="N16" s="33"/>
-      <c r="O16" s="33">
-        <v>25</v>
-      </c>
-      <c r="P16" s="51">
-        <v>3.1536000000000002E-2</v>
-      </c>
-      <c r="Q16" s="33"/>
-      <c r="R16" s="33"/>
-      <c r="S16" s="51">
-        <v>0.37</v>
-      </c>
-      <c r="T16" s="51">
-        <v>100</v>
-      </c>
-      <c r="U16" s="51">
-        <v>1</v>
-      </c>
-      <c r="V16" s="51"/>
-    </row>
-    <row r="17" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="P16" s="50"/>
+    </row>
+    <row r="17" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B17" s="18" t="s">
-        <v>131</v>
+        <v>119</v>
       </c>
       <c r="C17" s="18" t="s">
-        <v>132</v>
+        <v>120</v>
       </c>
       <c r="D17" s="18" t="s">
-        <v>133</v>
+        <v>121</v>
       </c>
       <c r="E17" s="18" t="s">
-        <v>96</v>
+        <v>84</v>
       </c>
       <c r="F17" s="18"/>
       <c r="G17" s="18"/>
-      <c r="H17" s="18"/>
-      <c r="I17" s="18">
+      <c r="H17" s="18">
         <v>1</v>
       </c>
+      <c r="I17" s="50"/>
       <c r="J17" s="18"/>
-      <c r="K17" s="18"/>
-      <c r="L17" s="51"/>
+      <c r="K17" s="50"/>
+      <c r="L17" s="18"/>
       <c r="M17" s="18"/>
       <c r="N17" s="18"/>
-      <c r="O17" s="51"/>
-      <c r="P17" s="18"/>
-      <c r="Q17" s="18"/>
-      <c r="R17" s="51"/>
-      <c r="S17" s="18"/>
-      <c r="T17" s="18"/>
-      <c r="U17" s="51"/>
-      <c r="V17" s="51"/>
-    </row>
-    <row r="18" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="O17" s="50"/>
+      <c r="P17" s="50"/>
+    </row>
+    <row r="18" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B18" s="18" t="s">
-        <v>134</v>
+        <v>122</v>
       </c>
       <c r="C18" s="18" t="s">
-        <v>135</v>
+        <v>123</v>
       </c>
       <c r="D18" s="18" t="s">
-        <v>136</v>
+        <v>124</v>
       </c>
       <c r="E18" s="18" t="s">
-        <v>99</v>
+        <v>87</v>
       </c>
       <c r="F18" s="18"/>
       <c r="G18" s="18"/>
-      <c r="H18" s="18"/>
-      <c r="I18" s="18">
+      <c r="H18" s="18">
         <v>1</v>
       </c>
+      <c r="I18" s="50"/>
       <c r="J18" s="18"/>
-      <c r="K18" s="18"/>
-      <c r="L18" s="51"/>
+      <c r="K18" s="50"/>
+      <c r="L18" s="18"/>
       <c r="M18" s="18"/>
       <c r="N18" s="18"/>
-      <c r="O18" s="51"/>
-      <c r="P18" s="18"/>
-      <c r="Q18" s="18"/>
-      <c r="R18" s="51"/>
-      <c r="S18" s="18"/>
-      <c r="T18" s="18"/>
-      <c r="U18" s="51"/>
-      <c r="V18" s="51"/>
-    </row>
-    <row r="19" spans="2:22" ht="24.6" x14ac:dyDescent="0.4">
+      <c r="O18" s="50"/>
+      <c r="P18" s="50"/>
+    </row>
+    <row r="19" spans="2:16" ht="24.6" x14ac:dyDescent="0.4">
       <c r="B19" s="32" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="22" spans="2:22" x14ac:dyDescent="0.25">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="22" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B22" s="22" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="23" spans="2:22" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="23" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B23" s="21" t="s">
         <v>0</v>
       </c>
       <c r="C23" s="21" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="D23" s="21" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="E23" s="21" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="F23" s="1"/>
     </row>
-    <row r="24" spans="2:22" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:16" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B24" s="19" t="s">
         <v>47</v>
       </c>
@@ -3262,37 +3112,37 @@
         <v>48</v>
       </c>
     </row>
-    <row r="25" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B25" s="23"/>
       <c r="C25" s="23"/>
       <c r="D25" s="23"/>
       <c r="E25" s="23"/>
     </row>
-    <row r="26" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B26" s="18"/>
       <c r="C26" s="18"/>
       <c r="D26" s="18"/>
       <c r="E26" s="18"/>
     </row>
-    <row r="27" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B27" s="18"/>
       <c r="C27" s="18"/>
       <c r="D27" s="18"/>
       <c r="E27" s="18"/>
     </row>
-    <row r="28" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B28" s="18"/>
       <c r="C28" s="18"/>
       <c r="D28" s="18"/>
       <c r="E28" s="18"/>
     </row>
-    <row r="29" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B29" s="18"/>
       <c r="C29" s="18"/>
       <c r="D29" s="18"/>
       <c r="E29" s="18"/>
     </row>
-    <row r="30" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B30" s="18"/>
       <c r="C30" s="18"/>
       <c r="D30" s="18"/>
@@ -3311,7 +3161,7 @@
   <dimension ref="A4:F12"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -3340,31 +3190,31 @@
         <v>0</v>
       </c>
       <c r="C7" s="17" t="s">
-        <v>88</v>
+        <v>76</v>
       </c>
       <c r="D7" s="17" t="s">
-        <v>96</v>
+        <v>84</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="C8" s="59" t="s">
-        <v>129</v>
-      </c>
-      <c r="D8" s="59" t="s">
-        <v>129</v>
+      <c r="C8" s="58" t="s">
+        <v>117</v>
+      </c>
+      <c r="D8" s="58" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B9" s="18" t="s">
-        <v>121</v>
-      </c>
-      <c r="C9" s="51">
+        <v>109</v>
+      </c>
+      <c r="C9" s="50">
         <v>94.6</v>
       </c>
-      <c r="D9" s="51">
+      <c r="D9" s="50">
         <v>57</v>
       </c>
     </row>

</xml_diff>

<commit_message>
CHPR = 2 to be the same as in the tutorial
</commit_message>
<xml_diff>
--- a/VT_SHR_ELC_V01.xlsx
+++ b/VT_SHR_ELC_V01.xlsx
@@ -1518,7 +1518,6 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="4" applyFont="1"/>
-    <xf numFmtId="2" fontId="4" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1572,6 +1571,7 @@
     <xf numFmtId="0" fontId="2" fillId="11" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="1" fontId="4" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2114,168 +2114,168 @@
       <c r="C4" s="24"/>
     </row>
     <row r="6" spans="2:10" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="B6" s="35" t="s">
+      <c r="B6" s="34" t="s">
         <v>43</v>
       </c>
-      <c r="C6" s="35"/>
-      <c r="D6" s="36"/>
-      <c r="E6" s="37"/>
-      <c r="F6" s="37"/>
-      <c r="G6" s="37"/>
-      <c r="H6" s="37"/>
-      <c r="I6" s="37"/>
-      <c r="J6" s="37"/>
+      <c r="C6" s="34"/>
+      <c r="D6" s="35"/>
+      <c r="E6" s="36"/>
+      <c r="F6" s="36"/>
+      <c r="G6" s="36"/>
+      <c r="H6" s="36"/>
+      <c r="I6" s="36"/>
+      <c r="J6" s="36"/>
     </row>
     <row r="7" spans="2:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="38" t="s">
+      <c r="B7" s="37" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="38"/>
-      <c r="D7" s="37"/>
-      <c r="E7" s="37"/>
-      <c r="F7" s="37"/>
-      <c r="G7" s="37"/>
-      <c r="H7" s="37"/>
-      <c r="I7" s="37"/>
-      <c r="J7" s="37"/>
+      <c r="C7" s="37"/>
+      <c r="D7" s="36"/>
+      <c r="E7" s="36"/>
+      <c r="F7" s="36"/>
+      <c r="G7" s="36"/>
+      <c r="H7" s="36"/>
+      <c r="I7" s="36"/>
+      <c r="J7" s="36"/>
     </row>
     <row r="8" spans="2:10" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="39" t="s">
+      <c r="B8" s="38" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="40" t="s">
+      <c r="C8" s="39" t="s">
         <v>32</v>
       </c>
-      <c r="D8" s="39" t="s">
+      <c r="D8" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="E8" s="39" t="s">
+      <c r="E8" s="38" t="s">
         <v>3</v>
       </c>
-      <c r="F8" s="41" t="s">
+      <c r="F8" s="40" t="s">
         <v>4</v>
       </c>
-      <c r="G8" s="41" t="s">
+      <c r="G8" s="40" t="s">
         <v>8</v>
       </c>
-      <c r="H8" s="41" t="s">
+      <c r="H8" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="I8" s="41" t="s">
+      <c r="I8" s="40" t="s">
         <v>10</v>
       </c>
-      <c r="J8" s="41" t="s">
+      <c r="J8" s="40" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="9" spans="2:10" ht="40.200000000000003" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="42" t="s">
+      <c r="B9" s="41" t="s">
         <v>50</v>
       </c>
-      <c r="C9" s="43" t="s">
+      <c r="C9" s="42" t="s">
         <v>33</v>
       </c>
-      <c r="D9" s="42" t="s">
+      <c r="D9" s="41" t="s">
         <v>28</v>
       </c>
-      <c r="E9" s="42" t="s">
+      <c r="E9" s="41" t="s">
         <v>29</v>
       </c>
-      <c r="F9" s="42" t="s">
+      <c r="F9" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="G9" s="42" t="s">
+      <c r="G9" s="41" t="s">
         <v>53</v>
       </c>
-      <c r="H9" s="42" t="s">
+      <c r="H9" s="41" t="s">
         <v>54</v>
       </c>
-      <c r="I9" s="42" t="s">
+      <c r="I9" s="41" t="s">
         <v>30</v>
       </c>
-      <c r="J9" s="42" t="s">
+      <c r="J9" s="41" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="10" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B10" s="50" t="s">
+      <c r="B10" s="49" t="s">
         <v>108</v>
       </c>
-      <c r="C10" s="57"/>
-      <c r="D10" s="50" t="s">
+      <c r="C10" s="56"/>
+      <c r="D10" s="49" t="s">
         <v>109</v>
       </c>
-      <c r="E10" s="50" t="s">
+      <c r="E10" s="49" t="s">
         <v>110</v>
       </c>
-      <c r="F10" s="50" t="s">
+      <c r="F10" s="49" t="s">
         <v>111</v>
       </c>
-      <c r="G10" s="50"/>
-      <c r="H10" s="50" t="s">
+      <c r="G10" s="49"/>
+      <c r="H10" s="49" t="s">
         <v>112</v>
       </c>
-      <c r="I10" s="50"/>
-      <c r="J10" s="50"/>
+      <c r="I10" s="49"/>
+      <c r="J10" s="49"/>
     </row>
     <row r="11" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B11" s="50" t="s">
+      <c r="B11" s="49" t="s">
         <v>113</v>
       </c>
-      <c r="C11" s="57"/>
-      <c r="D11" s="50" t="s">
+      <c r="C11" s="56"/>
+      <c r="D11" s="49" t="s">
         <v>76</v>
       </c>
-      <c r="E11" s="50" t="s">
+      <c r="E11" s="49" t="s">
         <v>114</v>
       </c>
-      <c r="F11" s="50" t="s">
+      <c r="F11" s="49" t="s">
         <v>102</v>
       </c>
-      <c r="G11" s="50" t="s">
+      <c r="G11" s="49" t="s">
         <v>105</v>
       </c>
-      <c r="H11" s="50"/>
-      <c r="I11" s="50"/>
-      <c r="J11" s="50"/>
+      <c r="H11" s="49"/>
+      <c r="I11" s="49"/>
+      <c r="J11" s="49"/>
     </row>
     <row r="12" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B12" s="50" t="s">
+      <c r="B12" s="49" t="s">
         <v>113</v>
       </c>
-      <c r="C12" s="57"/>
-      <c r="D12" s="50" t="s">
+      <c r="C12" s="56"/>
+      <c r="D12" s="49" t="s">
         <v>84</v>
       </c>
-      <c r="E12" s="50" t="s">
+      <c r="E12" s="49" t="s">
         <v>115</v>
       </c>
-      <c r="F12" s="50" t="s">
+      <c r="F12" s="49" t="s">
         <v>102</v>
       </c>
-      <c r="G12" s="50"/>
-      <c r="H12" s="50"/>
-      <c r="I12" s="50"/>
-      <c r="J12" s="50"/>
+      <c r="G12" s="49"/>
+      <c r="H12" s="49"/>
+      <c r="I12" s="49"/>
+      <c r="J12" s="49"/>
     </row>
     <row r="13" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B13" s="50" t="s">
+      <c r="B13" s="49" t="s">
         <v>113</v>
       </c>
-      <c r="C13" s="57"/>
-      <c r="D13" s="50" t="s">
+      <c r="C13" s="56"/>
+      <c r="D13" s="49" t="s">
         <v>87</v>
       </c>
-      <c r="E13" s="50" t="s">
+      <c r="E13" s="49" t="s">
         <v>116</v>
       </c>
-      <c r="F13" s="50" t="s">
+      <c r="F13" s="49" t="s">
         <v>102</v>
       </c>
-      <c r="G13" s="50"/>
-      <c r="H13" s="50"/>
-      <c r="I13" s="50"/>
-      <c r="J13" s="50"/>
+      <c r="G13" s="49"/>
+      <c r="H13" s="49"/>
+      <c r="I13" s="49"/>
+      <c r="J13" s="49"/>
     </row>
   </sheetData>
   <phoneticPr fontId="0" type="noConversion"/>
@@ -2321,245 +2321,245 @@
     </row>
     <row r="5" spans="1:10" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="12"/>
-      <c r="B5" s="35" t="s">
+      <c r="B5" s="34" t="s">
         <v>44</v>
       </c>
-      <c r="C5" s="44"/>
-      <c r="D5" s="44"/>
-      <c r="E5" s="44"/>
-      <c r="F5" s="44"/>
-      <c r="G5" s="44"/>
-      <c r="H5" s="44"/>
-      <c r="I5" s="44"/>
-      <c r="J5" s="44"/>
+      <c r="C5" s="43"/>
+      <c r="D5" s="43"/>
+      <c r="E5" s="43"/>
+      <c r="F5" s="43"/>
+      <c r="G5" s="43"/>
+      <c r="H5" s="43"/>
+      <c r="I5" s="43"/>
+      <c r="J5" s="43"/>
     </row>
     <row r="6" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="38" t="s">
+      <c r="B6" s="37" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="38"/>
-      <c r="D6" s="44"/>
-      <c r="E6" s="44"/>
-      <c r="F6" s="44"/>
-      <c r="G6" s="44"/>
-      <c r="H6" s="44"/>
-      <c r="I6" s="44"/>
-      <c r="J6" s="44"/>
+      <c r="C6" s="37"/>
+      <c r="D6" s="43"/>
+      <c r="E6" s="43"/>
+      <c r="F6" s="43"/>
+      <c r="G6" s="43"/>
+      <c r="H6" s="43"/>
+      <c r="I6" s="43"/>
+      <c r="J6" s="43"/>
     </row>
     <row r="7" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="40" t="s">
+      <c r="B7" s="39" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="40" t="s">
+      <c r="C7" s="39" t="s">
         <v>32</v>
       </c>
-      <c r="D7" s="40" t="s">
+      <c r="D7" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="E7" s="40" t="s">
+      <c r="E7" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="F7" s="40" t="s">
+      <c r="F7" s="39" t="s">
         <v>18</v>
       </c>
-      <c r="G7" s="40" t="s">
+      <c r="G7" s="39" t="s">
         <v>19</v>
       </c>
-      <c r="H7" s="40" t="s">
+      <c r="H7" s="39" t="s">
         <v>20</v>
       </c>
-      <c r="I7" s="40" t="s">
+      <c r="I7" s="39" t="s">
         <v>21</v>
       </c>
-      <c r="J7" s="40" t="s">
+      <c r="J7" s="39" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="40.200000000000003" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="43" t="s">
+      <c r="B8" s="42" t="s">
         <v>51</v>
       </c>
-      <c r="C8" s="43" t="s">
+      <c r="C8" s="42" t="s">
         <v>33</v>
       </c>
-      <c r="D8" s="43" t="s">
+      <c r="D8" s="42" t="s">
         <v>23</v>
       </c>
-      <c r="E8" s="43" t="s">
+      <c r="E8" s="42" t="s">
         <v>24</v>
       </c>
-      <c r="F8" s="43" t="s">
+      <c r="F8" s="42" t="s">
         <v>25</v>
       </c>
-      <c r="G8" s="43" t="s">
+      <c r="G8" s="42" t="s">
         <v>26</v>
       </c>
-      <c r="H8" s="43" t="s">
+      <c r="H8" s="42" t="s">
         <v>57</v>
       </c>
-      <c r="I8" s="43" t="s">
+      <c r="I8" s="42" t="s">
         <v>56</v>
       </c>
-      <c r="J8" s="43" t="s">
+      <c r="J8" s="42" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B9" s="57" t="s">
+      <c r="B9" s="56" t="s">
         <v>100</v>
       </c>
-      <c r="C9" s="57"/>
-      <c r="D9" s="57" t="s">
+      <c r="C9" s="56"/>
+      <c r="D9" s="56" t="s">
         <v>77</v>
       </c>
-      <c r="E9" s="57" t="s">
+      <c r="E9" s="56" t="s">
         <v>101</v>
       </c>
-      <c r="F9" s="57" t="s">
+      <c r="F9" s="56" t="s">
         <v>102</v>
       </c>
-      <c r="G9" s="57" t="s">
+      <c r="G9" s="56" t="s">
         <v>99</v>
       </c>
-      <c r="H9" s="57"/>
-      <c r="I9" s="57"/>
-      <c r="J9" s="57"/>
+      <c r="H9" s="56"/>
+      <c r="I9" s="56"/>
+      <c r="J9" s="56"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B10" s="57" t="s">
+      <c r="B10" s="56" t="s">
         <v>103</v>
       </c>
-      <c r="C10" s="57"/>
-      <c r="D10" s="57" t="s">
+      <c r="C10" s="56"/>
+      <c r="D10" s="56" t="s">
         <v>73</v>
       </c>
-      <c r="E10" s="57" t="s">
+      <c r="E10" s="56" t="s">
         <v>74</v>
       </c>
-      <c r="F10" s="57" t="s">
+      <c r="F10" s="56" t="s">
         <v>102</v>
       </c>
-      <c r="G10" s="57" t="s">
+      <c r="G10" s="56" t="s">
         <v>104</v>
       </c>
-      <c r="H10" s="57" t="s">
+      <c r="H10" s="56" t="s">
         <v>105</v>
       </c>
-      <c r="I10" s="57"/>
-      <c r="J10" s="57"/>
+      <c r="I10" s="56"/>
+      <c r="J10" s="56"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B11" s="57" t="s">
+      <c r="B11" s="56" t="s">
         <v>106</v>
       </c>
-      <c r="C11" s="57"/>
-      <c r="D11" s="57" t="s">
+      <c r="C11" s="56"/>
+      <c r="D11" s="56" t="s">
         <v>118</v>
       </c>
-      <c r="E11" s="57" t="s">
+      <c r="E11" s="56" t="s">
         <v>80</v>
       </c>
-      <c r="F11" s="57" t="s">
+      <c r="F11" s="56" t="s">
         <v>102</v>
       </c>
-      <c r="G11" s="57" t="s">
+      <c r="G11" s="56" t="s">
         <v>99</v>
       </c>
-      <c r="H11" s="57"/>
-      <c r="I11" s="57"/>
-      <c r="J11" s="57"/>
+      <c r="H11" s="56"/>
+      <c r="I11" s="56"/>
+      <c r="J11" s="56"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B12" s="57" t="s">
+      <c r="B12" s="56" t="s">
         <v>107</v>
       </c>
-      <c r="C12" s="57"/>
-      <c r="D12" s="57" t="s">
+      <c r="C12" s="56"/>
+      <c r="D12" s="56" t="s">
         <v>82</v>
       </c>
-      <c r="E12" s="57" t="s">
+      <c r="E12" s="56" t="s">
         <v>83</v>
       </c>
-      <c r="F12" s="57" t="s">
+      <c r="F12" s="56" t="s">
         <v>102</v>
       </c>
-      <c r="G12" s="57" t="s">
+      <c r="G12" s="56" t="s">
         <v>99</v>
       </c>
-      <c r="H12" s="57"/>
-      <c r="I12" s="57"/>
-      <c r="J12" s="57"/>
+      <c r="H12" s="56"/>
+      <c r="I12" s="56"/>
+      <c r="J12" s="56"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B13" s="57" t="s">
+      <c r="B13" s="56" t="s">
         <v>107</v>
       </c>
-      <c r="C13" s="57"/>
-      <c r="D13" s="57" t="s">
+      <c r="C13" s="56"/>
+      <c r="D13" s="56" t="s">
         <v>85</v>
       </c>
-      <c r="E13" s="57" t="s">
+      <c r="E13" s="56" t="s">
         <v>86</v>
       </c>
-      <c r="F13" s="57" t="s">
+      <c r="F13" s="56" t="s">
         <v>102</v>
       </c>
-      <c r="G13" s="57" t="s">
+      <c r="G13" s="56" t="s">
         <v>99</v>
       </c>
-      <c r="H13" s="57"/>
-      <c r="I13" s="57"/>
-      <c r="J13" s="57"/>
+      <c r="H13" s="56"/>
+      <c r="I13" s="56"/>
+      <c r="J13" s="56"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B14" s="57" t="s">
+      <c r="B14" s="56" t="s">
         <v>103</v>
       </c>
-      <c r="C14" s="57"/>
-      <c r="D14" s="57" t="str">
+      <c r="C14" s="56"/>
+      <c r="D14" s="56" t="str">
         <f>ProcessCharac!B17</f>
         <v>FT-ELCNGA</v>
       </c>
-      <c r="E14" s="57" t="str">
+      <c r="E14" s="56" t="str">
         <f>ProcessCharac!C17</f>
         <v>Fuel Technology Natural Gas ELC</v>
       </c>
-      <c r="F14" s="57" t="s">
+      <c r="F14" s="56" t="s">
         <v>102</v>
       </c>
-      <c r="G14" s="57" t="s">
+      <c r="G14" s="56" t="s">
         <v>104</v>
       </c>
-      <c r="H14" s="57" t="s">
+      <c r="H14" s="56" t="s">
         <v>105</v>
       </c>
-      <c r="I14" s="57"/>
-      <c r="J14" s="57"/>
+      <c r="I14" s="56"/>
+      <c r="J14" s="56"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B15" s="57" t="s">
+      <c r="B15" s="56" t="s">
         <v>103</v>
       </c>
-      <c r="C15" s="57"/>
-      <c r="D15" s="57" t="str">
+      <c r="C15" s="56"/>
+      <c r="D15" s="56" t="str">
         <f>ProcessCharac!B18</f>
         <v>FT-ELCWIN</v>
       </c>
-      <c r="E15" s="57" t="str">
+      <c r="E15" s="56" t="str">
         <f>ProcessCharac!C18</f>
         <v>Fuel Technology Wind ELC</v>
       </c>
-      <c r="F15" s="57" t="s">
+      <c r="F15" s="56" t="s">
         <v>102</v>
       </c>
-      <c r="G15" s="57" t="s">
+      <c r="G15" s="56" t="s">
         <v>104</v>
       </c>
-      <c r="H15" s="57" t="s">
+      <c r="H15" s="56" t="s">
         <v>105</v>
       </c>
-      <c r="I15" s="57"/>
-      <c r="J15" s="57"/>
+      <c r="I15" s="56"/>
+      <c r="J15" s="56"/>
     </row>
   </sheetData>
   <phoneticPr fontId="0" type="noConversion"/>
@@ -2575,7 +2575,7 @@
   <dimension ref="B1:S30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="Q12" sqref="Q12"/>
+      <selection activeCell="N23" sqref="N23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -2663,133 +2663,133 @@
       <c r="R7" s="27"/>
     </row>
     <row r="8" spans="2:19" s="1" customFormat="1" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="46" t="s">
+      <c r="B8" s="45" t="s">
         <v>1</v>
       </c>
-      <c r="C8" s="47" t="s">
+      <c r="C8" s="46" t="s">
         <v>49</v>
       </c>
-      <c r="D8" s="46" t="s">
+      <c r="D8" s="45" t="s">
         <v>5</v>
       </c>
-      <c r="E8" s="46" t="s">
+      <c r="E8" s="45" t="s">
         <v>6</v>
       </c>
-      <c r="F8" s="46" t="s">
+      <c r="F8" s="45" t="s">
         <v>69</v>
       </c>
-      <c r="G8" s="46" t="s">
+      <c r="G8" s="45" t="s">
         <v>60</v>
       </c>
-      <c r="H8" s="34" t="s">
+      <c r="H8" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="I8" s="34" t="s">
+      <c r="I8" s="33" t="s">
         <v>65</v>
       </c>
-      <c r="J8" s="34" t="s">
+      <c r="J8" s="33" t="s">
         <v>63</v>
       </c>
-      <c r="K8" s="34" t="s">
+      <c r="K8" s="33" t="s">
         <v>71</v>
       </c>
-      <c r="L8" s="34" t="s">
+      <c r="L8" s="33" t="s">
         <v>64</v>
       </c>
-      <c r="M8" s="53" t="s">
+      <c r="M8" s="52" t="s">
         <v>90</v>
       </c>
-      <c r="N8" s="53" t="s">
+      <c r="N8" s="52" t="s">
         <v>91</v>
       </c>
-      <c r="O8" s="53" t="s">
+      <c r="O8" s="52" t="s">
         <v>92</v>
       </c>
-      <c r="P8" s="53" t="s">
+      <c r="P8" s="52" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="9" spans="2:19" ht="54.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="45" t="s">
+      <c r="B9" s="44" t="s">
         <v>52</v>
       </c>
-      <c r="C9" s="45" t="s">
+      <c r="C9" s="44" t="s">
         <v>24</v>
       </c>
-      <c r="D9" s="45" t="s">
+      <c r="D9" s="44" t="s">
         <v>37</v>
       </c>
-      <c r="E9" s="45" t="s">
+      <c r="E9" s="44" t="s">
         <v>38</v>
       </c>
-      <c r="F9" s="45" t="s">
+      <c r="F9" s="44" t="s">
         <v>69</v>
       </c>
-      <c r="G9" s="45" t="s">
+      <c r="G9" s="44" t="s">
         <v>70</v>
       </c>
-      <c r="H9" s="45" t="s">
+      <c r="H9" s="44" t="s">
         <v>39</v>
       </c>
-      <c r="I9" s="45" t="s">
+      <c r="I9" s="44" t="s">
         <v>46</v>
       </c>
-      <c r="J9" s="45" t="s">
+      <c r="J9" s="44" t="s">
         <v>45</v>
       </c>
-      <c r="K9" s="45" t="s">
+      <c r="K9" s="44" t="s">
         <v>72</v>
       </c>
-      <c r="L9" s="45" t="s">
+      <c r="L9" s="44" t="s">
         <v>40</v>
       </c>
-      <c r="M9" s="54" t="s">
+      <c r="M9" s="53" t="s">
         <v>94</v>
       </c>
-      <c r="N9" s="54" t="s">
+      <c r="N9" s="53" t="s">
         <v>95</v>
       </c>
-      <c r="O9" s="54" t="s">
+      <c r="O9" s="53" t="s">
         <v>96</v>
       </c>
-      <c r="P9" s="54" t="s">
+      <c r="P9" s="53" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="10" spans="2:19" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B10" s="48" t="s">
+      <c r="B10" s="47" t="s">
         <v>67</v>
       </c>
-      <c r="C10" s="49"/>
-      <c r="D10" s="49"/>
-      <c r="E10" s="49"/>
-      <c r="F10" s="48"/>
-      <c r="G10" s="48" t="s">
+      <c r="C10" s="48"/>
+      <c r="D10" s="48"/>
+      <c r="E10" s="48"/>
+      <c r="F10" s="47"/>
+      <c r="G10" s="47" t="s">
         <v>70</v>
       </c>
-      <c r="H10" s="48" t="s">
+      <c r="H10" s="47" t="s">
         <v>98</v>
       </c>
-      <c r="I10" s="48" t="s">
+      <c r="I10" s="47" t="s">
         <v>125</v>
       </c>
-      <c r="J10" s="48" t="s">
+      <c r="J10" s="47" t="s">
         <v>126</v>
       </c>
-      <c r="K10" s="49" t="s">
+      <c r="K10" s="48" t="s">
         <v>127</v>
       </c>
-      <c r="L10" s="48" t="s">
+      <c r="L10" s="47" t="s">
         <v>98</v>
       </c>
-      <c r="M10" s="55" t="s">
+      <c r="M10" s="54" t="s">
         <v>98</v>
       </c>
-      <c r="N10" s="55" t="s">
+      <c r="N10" s="54" t="s">
         <v>99</v>
       </c>
-      <c r="O10" s="56"/>
-      <c r="P10" s="56"/>
+      <c r="O10" s="55"/>
+      <c r="P10" s="55"/>
     </row>
     <row r="11" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B11" s="18" t="s">
@@ -2809,14 +2809,14 @@
       <c r="H11" s="18">
         <v>1</v>
       </c>
-      <c r="I11" s="50"/>
-      <c r="J11" s="50"/>
+      <c r="I11" s="49"/>
+      <c r="J11" s="49"/>
       <c r="K11" s="18"/>
-      <c r="L11" s="50"/>
-      <c r="M11" s="50"/>
-      <c r="N11" s="50"/>
-      <c r="O11" s="50"/>
-      <c r="P11" s="50"/>
+      <c r="L11" s="49"/>
+      <c r="M11" s="49"/>
+      <c r="N11" s="49"/>
+      <c r="O11" s="49"/>
+      <c r="P11" s="49"/>
     </row>
     <row r="12" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B12" s="18" t="s">
@@ -2840,28 +2840,28 @@
       <c r="H12" s="18">
         <v>0.437</v>
       </c>
-      <c r="I12" s="50">
+      <c r="I12" s="49">
         <v>2.145E-2</v>
       </c>
-      <c r="J12" s="50">
+      <c r="J12" s="49">
         <v>0.93089999999999995</v>
       </c>
       <c r="K12" s="18">
         <v>40</v>
       </c>
-      <c r="L12" s="50">
+      <c r="L12" s="49">
         <v>3.1536000000000002E-2</v>
       </c>
-      <c r="M12" s="50">
+      <c r="M12" s="49">
         <v>0.85099999999999998</v>
       </c>
-      <c r="N12" s="50">
+      <c r="N12" s="49">
         <v>108.2</v>
       </c>
-      <c r="O12" s="50">
+      <c r="O12" s="49">
         <v>1</v>
       </c>
-      <c r="P12" s="50"/>
+      <c r="P12" s="49"/>
     </row>
     <row r="13" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B13" s="18" t="s">
@@ -2885,29 +2885,29 @@
       <c r="H13" s="18">
         <v>0.28000000000000003</v>
       </c>
-      <c r="I13" s="51">
+      <c r="I13" s="50">
         <v>0.1</v>
       </c>
-      <c r="J13" s="51">
+      <c r="J13" s="50">
         <v>0.6</v>
       </c>
       <c r="K13" s="18">
         <v>35</v>
       </c>
-      <c r="L13" s="50">
+      <c r="L13" s="49">
         <v>3.1536000000000002E-2</v>
       </c>
-      <c r="M13" s="50">
+      <c r="M13" s="49">
         <v>0.86</v>
       </c>
-      <c r="N13" s="50">
+      <c r="N13" s="49">
         <v>90000</v>
       </c>
-      <c r="O13" s="50">
+      <c r="O13" s="49">
         <v>1</v>
       </c>
-      <c r="P13" s="50">
-        <v>2.1</v>
+      <c r="P13" s="49">
+        <v>2</v>
       </c>
     </row>
     <row r="14" spans="2:19" x14ac:dyDescent="0.25">
@@ -2920,14 +2920,14 @@
       <c r="F14" s="18"/>
       <c r="G14" s="18"/>
       <c r="H14" s="18"/>
-      <c r="I14" s="50"/>
-      <c r="J14" s="50"/>
+      <c r="I14" s="49"/>
+      <c r="J14" s="49"/>
       <c r="K14" s="18"/>
-      <c r="L14" s="50"/>
-      <c r="M14" s="50"/>
-      <c r="N14" s="50"/>
-      <c r="O14" s="50"/>
-      <c r="P14" s="50"/>
+      <c r="L14" s="49"/>
+      <c r="M14" s="49"/>
+      <c r="N14" s="49"/>
+      <c r="O14" s="49"/>
+      <c r="P14" s="49"/>
     </row>
     <row r="15" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B15" s="18" t="s">
@@ -2951,28 +2951,28 @@
       <c r="H15" s="18">
         <v>0.39</v>
       </c>
-      <c r="I15" s="50">
+      <c r="I15" s="49">
         <v>0.02</v>
       </c>
-      <c r="J15" s="50">
+      <c r="J15" s="49">
         <v>1.25</v>
       </c>
       <c r="K15" s="18">
         <v>25</v>
       </c>
-      <c r="L15" s="50">
+      <c r="L15" s="49">
         <v>3.1536000000000002E-2</v>
       </c>
-      <c r="M15" s="51">
+      <c r="M15" s="50">
         <v>0.92346153799999997</v>
       </c>
-      <c r="N15" s="50">
+      <c r="N15" s="49">
         <v>100</v>
       </c>
-      <c r="O15" s="50">
+      <c r="O15" s="49">
         <v>1</v>
       </c>
-      <c r="P15" s="50"/>
+      <c r="P15" s="49"/>
     </row>
     <row r="16" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B16" s="18" t="s">
@@ -2996,28 +2996,28 @@
       <c r="H16" s="18">
         <v>1</v>
       </c>
-      <c r="I16" s="52">
+      <c r="I16" s="51">
         <v>2.5599999999999998E-2</v>
       </c>
-      <c r="J16" s="52">
+      <c r="J16" s="51">
         <v>0.77777777777777779</v>
       </c>
-      <c r="K16" s="33">
+      <c r="K16" s="58">
         <v>25</v>
       </c>
-      <c r="L16" s="50">
+      <c r="L16" s="49">
         <v>3.1536000000000002E-2</v>
       </c>
-      <c r="M16" s="50">
+      <c r="M16" s="49">
         <v>0.37</v>
       </c>
-      <c r="N16" s="50">
+      <c r="N16" s="49">
         <v>100</v>
       </c>
-      <c r="O16" s="50">
+      <c r="O16" s="49">
         <v>1</v>
       </c>
-      <c r="P16" s="50"/>
+      <c r="P16" s="49"/>
     </row>
     <row r="17" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B17" s="18" t="s">
@@ -3037,14 +3037,14 @@
       <c r="H17" s="18">
         <v>1</v>
       </c>
-      <c r="I17" s="50"/>
+      <c r="I17" s="49"/>
       <c r="J17" s="18"/>
-      <c r="K17" s="50"/>
+      <c r="K17" s="49"/>
       <c r="L17" s="18"/>
       <c r="M17" s="18"/>
       <c r="N17" s="18"/>
-      <c r="O17" s="50"/>
-      <c r="P17" s="50"/>
+      <c r="O17" s="49"/>
+      <c r="P17" s="49"/>
     </row>
     <row r="18" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B18" s="18" t="s">
@@ -3064,14 +3064,14 @@
       <c r="H18" s="18">
         <v>1</v>
       </c>
-      <c r="I18" s="50"/>
+      <c r="I18" s="49"/>
       <c r="J18" s="18"/>
-      <c r="K18" s="50"/>
+      <c r="K18" s="49"/>
       <c r="L18" s="18"/>
       <c r="M18" s="18"/>
       <c r="N18" s="18"/>
-      <c r="O18" s="50"/>
-      <c r="P18" s="50"/>
+      <c r="O18" s="49"/>
+      <c r="P18" s="49"/>
     </row>
     <row r="19" spans="2:16" ht="24.6" x14ac:dyDescent="0.4">
       <c r="B19" s="32" t="s">
@@ -3098,7 +3098,7 @@
       </c>
       <c r="F23" s="1"/>
     </row>
-    <row r="24" spans="2:16" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:16" ht="40.200000000000003" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B24" s="19" t="s">
         <v>47</v>
       </c>
@@ -3200,10 +3200,10 @@
       <c r="B8" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="C8" s="58" t="s">
+      <c r="C8" s="57" t="s">
         <v>117</v>
       </c>
-      <c r="D8" s="58" t="s">
+      <c r="D8" s="57" t="s">
         <v>117</v>
       </c>
     </row>
@@ -3211,10 +3211,10 @@
       <c r="B9" s="18" t="s">
         <v>109</v>
       </c>
-      <c r="C9" s="50">
+      <c r="C9" s="49">
         <v>94.6</v>
       </c>
-      <c r="D9" s="50">
+      <c r="D9" s="49">
         <v>57</v>
       </c>
     </row>

</xml_diff>

<commit_message>
New value for the backpressure plant installed capacity
</commit_message>
<xml_diff>
--- a/VT_SHR_ELC_V01.xlsx
+++ b/VT_SHR_ELC_V01.xlsx
@@ -2082,7 +2082,7 @@
   <dimension ref="B1:J13"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G30" sqref="G30"/>
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -2575,7 +2575,7 @@
   <dimension ref="B1:S30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="N23" sqref="N23"/>
+      <selection activeCell="K38" sqref="K38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -2901,7 +2901,7 @@
         <v>0.86</v>
       </c>
       <c r="N13" s="49">
-        <v>90000</v>
+        <v>100000</v>
       </c>
       <c r="O13" s="49">
         <v>1</v>
@@ -3161,7 +3161,7 @@
   <dimension ref="A4:F12"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+      <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Installed capacity for the BP plant has been increased from 90 GW to 100 GW, according to the exercise
</commit_message>
<xml_diff>
--- a/VT_SHR_ELC_V01.xlsx
+++ b/VT_SHR_ELC_V01.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="9552" yWindow="-12" windowWidth="4128" windowHeight="9408" tabRatio="901" activeTab="2"/>
+    <workbookView xWindow="9552" yWindow="-12" windowWidth="4128" windowHeight="9408" tabRatio="901"/>
   </bookViews>
   <sheets>
     <sheet name="SEC_Comm" sheetId="112" r:id="rId1"/>
@@ -2081,8 +2081,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="B1:J13"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G30" sqref="G30"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -2291,7 +2291,7 @@
   <dimension ref="A1:J15"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -2574,8 +2574,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:S30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="N23" sqref="N23"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="R32" sqref="R32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -2901,7 +2901,7 @@
         <v>0.86</v>
       </c>
       <c r="N13" s="49">
-        <v>90000</v>
+        <v>100000</v>
       </c>
       <c r="O13" s="49">
         <v>1</v>

</xml_diff>

<commit_message>
I have changed the numbers in the cells so that they are different than what the students have on Monday (after the end of the transportation lecture). Then I have deleted the value from some cells and the students have to find the right values. I still have to change something in the industrial sector
</commit_message>
<xml_diff>
--- a/VT_SHR_ELC_V01.xlsx
+++ b/VT_SHR_ELC_V01.xlsx
@@ -5,11 +5,11 @@
   <workbookPr showObjects="placeholders" codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Najub\TIMES-Shire\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VEDA\VEDA_Models\~g2v_TIMES-Shire\Course_Calibration\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="9552" yWindow="-12" windowWidth="4128" windowHeight="9408" tabRatio="901"/>
+    <workbookView xWindow="9552" yWindow="-12" windowWidth="4128" windowHeight="9408" tabRatio="901" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="SEC_Comm" sheetId="112" r:id="rId1"/>
@@ -1316,7 +1316,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="13">
+  <fills count="16">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1389,6 +1389,24 @@
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="5">
     <border>
@@ -1448,7 +1466,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1572,6 +1590,11 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="1" fontId="4" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="4" fillId="15" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="4" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2081,7 +2104,7 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="B1:J13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
@@ -2574,8 +2597,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:S30"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="R32" sqref="R32"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="P13" sqref="P13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -2837,8 +2860,8 @@
       <c r="G12" s="18" t="s">
         <v>88</v>
       </c>
-      <c r="H12" s="18">
-        <v>0.437</v>
+      <c r="H12" s="60">
+        <v>0.42099999999999999</v>
       </c>
       <c r="I12" s="49">
         <v>2.145E-2</v>
@@ -2852,11 +2875,11 @@
       <c r="L12" s="49">
         <v>3.1536000000000002E-2</v>
       </c>
-      <c r="M12" s="49">
-        <v>0.85099999999999998</v>
-      </c>
-      <c r="N12" s="49">
-        <v>108.2</v>
+      <c r="M12" s="61">
+        <v>0.872</v>
+      </c>
+      <c r="N12" s="61">
+        <v>261.39999999999998</v>
       </c>
       <c r="O12" s="49">
         <v>1</v>
@@ -2882,8 +2905,8 @@
       <c r="G13" s="18" t="s">
         <v>88</v>
       </c>
-      <c r="H13" s="18">
-        <v>0.28000000000000003</v>
+      <c r="H13" s="60">
+        <v>0.34</v>
       </c>
       <c r="I13" s="50">
         <v>0.1</v>
@@ -2897,18 +2920,14 @@
       <c r="L13" s="49">
         <v>3.1536000000000002E-2</v>
       </c>
-      <c r="M13" s="49">
-        <v>0.86</v>
-      </c>
-      <c r="N13" s="49">
-        <v>100000</v>
-      </c>
+      <c r="M13" s="61">
+        <v>0.85</v>
+      </c>
+      <c r="N13" s="63"/>
       <c r="O13" s="49">
         <v>1</v>
       </c>
-      <c r="P13" s="49">
-        <v>2</v>
-      </c>
+      <c r="P13" s="59"/>
     </row>
     <row r="14" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B14" s="18"/>
@@ -2948,8 +2967,8 @@
       <c r="G15" s="18" t="s">
         <v>89</v>
       </c>
-      <c r="H15" s="18">
-        <v>0.39</v>
+      <c r="H15" s="60">
+        <v>0.44</v>
       </c>
       <c r="I15" s="49">
         <v>0.02</v>
@@ -2963,11 +2982,11 @@
       <c r="L15" s="49">
         <v>3.1536000000000002E-2</v>
       </c>
-      <c r="M15" s="50">
-        <v>0.92346153799999997</v>
-      </c>
-      <c r="N15" s="49">
-        <v>100</v>
+      <c r="M15" s="62">
+        <v>0.91</v>
+      </c>
+      <c r="N15" s="61">
+        <v>237</v>
       </c>
       <c r="O15" s="49">
         <v>1</v>
@@ -3008,11 +3027,9 @@
       <c r="L16" s="49">
         <v>3.1536000000000002E-2</v>
       </c>
-      <c r="M16" s="49">
-        <v>0.37</v>
-      </c>
-      <c r="N16" s="49">
-        <v>100</v>
+      <c r="M16" s="59"/>
+      <c r="N16" s="61">
+        <v>562</v>
       </c>
       <c r="O16" s="49">
         <v>1</v>

</xml_diff>

<commit_message>
Exercise for lecture on calibration with solutions
</commit_message>
<xml_diff>
--- a/VT_SHR_ELC_V01.xlsx
+++ b/VT_SHR_ELC_V01.xlsx
@@ -1316,7 +1316,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="16">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1397,13 +1397,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF92D050"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF92D050"/>
+        <fgColor theme="0" tint="-0.249977111117893"/>
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
@@ -1466,7 +1460,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="64">
+  <cellXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1591,10 +1585,11 @@
     </xf>
     <xf numFmtId="1" fontId="4" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="4" fillId="15" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="4" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="4" fillId="14" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="4" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2597,8 +2592,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:S30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="P13" sqref="P13"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="M16" sqref="M16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -2860,7 +2855,7 @@
       <c r="G12" s="18" t="s">
         <v>88</v>
       </c>
-      <c r="H12" s="60">
+      <c r="H12" s="61">
         <v>0.42099999999999999</v>
       </c>
       <c r="I12" s="49">
@@ -2875,10 +2870,10 @@
       <c r="L12" s="49">
         <v>3.1536000000000002E-2</v>
       </c>
-      <c r="M12" s="61">
+      <c r="M12" s="62">
         <v>0.872</v>
       </c>
-      <c r="N12" s="61">
+      <c r="N12" s="62">
         <v>261.39999999999998</v>
       </c>
       <c r="O12" s="49">
@@ -2905,7 +2900,7 @@
       <c r="G13" s="18" t="s">
         <v>88</v>
       </c>
-      <c r="H13" s="60">
+      <c r="H13" s="61">
         <v>0.34</v>
       </c>
       <c r="I13" s="50">
@@ -2920,14 +2915,18 @@
       <c r="L13" s="49">
         <v>3.1536000000000002E-2</v>
       </c>
-      <c r="M13" s="61">
+      <c r="M13" s="62">
         <v>0.85</v>
       </c>
-      <c r="N13" s="63"/>
+      <c r="N13" s="60">
+        <v>809.53233652669599</v>
+      </c>
       <c r="O13" s="49">
         <v>1</v>
       </c>
-      <c r="P13" s="59"/>
+      <c r="P13" s="59">
+        <v>2</v>
+      </c>
     </row>
     <row r="14" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B14" s="18"/>
@@ -2938,12 +2937,12 @@
       </c>
       <c r="F14" s="18"/>
       <c r="G14" s="18"/>
-      <c r="H14" s="18"/>
+      <c r="H14" s="61"/>
       <c r="I14" s="49"/>
       <c r="J14" s="49"/>
       <c r="K14" s="18"/>
       <c r="L14" s="49"/>
-      <c r="M14" s="49"/>
+      <c r="M14" s="62"/>
       <c r="N14" s="49"/>
       <c r="O14" s="49"/>
       <c r="P14" s="49"/>
@@ -2967,7 +2966,7 @@
       <c r="G15" s="18" t="s">
         <v>89</v>
       </c>
-      <c r="H15" s="60">
+      <c r="H15" s="61">
         <v>0.44</v>
       </c>
       <c r="I15" s="49">
@@ -2982,10 +2981,10 @@
       <c r="L15" s="49">
         <v>3.1536000000000002E-2</v>
       </c>
-      <c r="M15" s="62">
+      <c r="M15" s="63">
         <v>0.91</v>
       </c>
-      <c r="N15" s="61">
+      <c r="N15" s="62">
         <v>237</v>
       </c>
       <c r="O15" s="49">
@@ -3012,7 +3011,7 @@
       <c r="G16" s="18" t="s">
         <v>89</v>
       </c>
-      <c r="H16" s="18">
+      <c r="H16" s="61">
         <v>1</v>
       </c>
       <c r="I16" s="51">
@@ -3027,8 +3026,10 @@
       <c r="L16" s="49">
         <v>3.1536000000000002E-2</v>
       </c>
-      <c r="M16" s="59"/>
-      <c r="N16" s="61">
+      <c r="M16" s="64">
+        <v>0.25999772501990598</v>
+      </c>
+      <c r="N16" s="62">
         <v>562</v>
       </c>
       <c r="O16" s="49">

</xml_diff>

<commit_message>
Delated all the cells that have to be refilled by students
</commit_message>
<xml_diff>
--- a/VT_SHR_ELC_V01.xlsx
+++ b/VT_SHR_ELC_V01.xlsx
@@ -2593,7 +2593,7 @@
   <dimension ref="B1:S30"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="M16" sqref="M16"/>
+      <selection activeCell="P13" sqref="P13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -2918,15 +2918,11 @@
       <c r="M13" s="62">
         <v>0.85</v>
       </c>
-      <c r="N13" s="60">
-        <v>809.53233652669599</v>
-      </c>
+      <c r="N13" s="60"/>
       <c r="O13" s="49">
         <v>1</v>
       </c>
-      <c r="P13" s="59">
-        <v>2</v>
-      </c>
+      <c r="P13" s="59"/>
     </row>
     <row r="14" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B14" s="18"/>
@@ -3026,9 +3022,7 @@
       <c r="L16" s="49">
         <v>3.1536000000000002E-2</v>
       </c>
-      <c r="M16" s="64">
-        <v>0.25999772501990598</v>
-      </c>
+      <c r="M16" s="64"/>
       <c r="N16" s="62">
         <v>562</v>
       </c>

</xml_diff>

<commit_message>
Just changed colour of a cell
</commit_message>
<xml_diff>
--- a/VT_SHR_ELC_V01.xlsx
+++ b/VT_SHR_ELC_V01.xlsx
@@ -5,7 +5,7 @@
   <workbookPr showObjects="placeholders" codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VEDA\VEDA_Models\~g2v_TIMES-Shire\Course_Calibration\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jactat\Documents\Models\TIMES-Shire\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -2592,7 +2592,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:S30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="M16" sqref="M16"/>
     </sheetView>
   </sheetViews>

</xml_diff>